<commit_message>
Atualizado por script em 01-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/indonesia_liga-1_2023-2024.xlsx
+++ b/2023/indonesia_liga-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V153"/>
+  <dimension ref="A1:V154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2413,22 +2413,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Persik Kediri</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Arema FC</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J22" t="n">
-        <v>1.71</v>
+        <v>2.52</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -2436,15 +2436,15 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>2.08</v>
+        <v>2.85</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>15/07/2023 09:52</t>
+          <t>15/07/2023 09:59</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.61</v>
+        <v>3.33</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2452,15 +2452,15 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.29</v>
+        <v>3.45</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>15/07/2023 09:52</t>
+          <t>15/07/2023 09:50</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>4.32</v>
+        <v>2.54</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -2468,16 +2468,16 @@
         </is>
       </c>
       <c r="T22" t="n">
-        <v>3.66</v>
+        <v>2.4</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>15/07/2023 09:52</t>
+          <t>15/07/2023 09:59</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-arema-fc/vXWQdmTf/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-persita/nczZfRc7/</t>
         </is>
       </c>
     </row>
@@ -2505,22 +2505,22 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>Arema FC</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" t="n">
-        <v>2.52</v>
+        <v>1.71</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -2528,15 +2528,15 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>2.85</v>
+        <v>2.08</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>15/07/2023 09:59</t>
+          <t>15/07/2023 09:52</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>3.33</v>
+        <v>3.61</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2544,15 +2544,15 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.45</v>
+        <v>3.29</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>15/07/2023 09:50</t>
+          <t>15/07/2023 09:52</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>2.54</v>
+        <v>4.32</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
@@ -2560,16 +2560,16 @@
         </is>
       </c>
       <c r="T23" t="n">
-        <v>2.4</v>
+        <v>3.66</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>15/07/2023 09:59</t>
+          <t>15/07/2023 09:52</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-persita/nczZfRc7/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-arema-fc/vXWQdmTf/</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Bali United</t>
+          <t>Persis Solo</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -2605,14 +2605,14 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Madura United</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="I24" t="n">
         <v>1</v>
       </c>
       <c r="J24" t="n">
-        <v>1.86</v>
+        <v>2.81</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
@@ -2620,15 +2620,15 @@
         </is>
       </c>
       <c r="L24" t="n">
-        <v>1.96</v>
+        <v>3</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>15/07/2023 13:58</t>
+          <t>15/07/2023 13:57</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>3.69</v>
+        <v>3.38</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2636,15 +2636,15 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>3.61</v>
+        <v>3.49</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>15/07/2023 13:58</t>
+          <t>15/07/2023 13:57</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>3.52</v>
+        <v>2.27</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -2652,16 +2652,16 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>3.7</v>
+        <v>2.29</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>15/07/2023 13:58</t>
+          <t>15/07/2023 13:57</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/bali-united-madura-united/INVUe7r1/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persis-solo-borneo/d8sMcTDl/</t>
         </is>
       </c>
     </row>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Persis Solo</t>
+          <t>Bali United</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -2697,14 +2697,14 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Madura United</t>
         </is>
       </c>
       <c r="I25" t="n">
         <v>1</v>
       </c>
       <c r="J25" t="n">
-        <v>2.81</v>
+        <v>1.86</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -2712,15 +2712,15 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>3</v>
+        <v>1.96</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>15/07/2023 13:57</t>
+          <t>15/07/2023 13:58</t>
         </is>
       </c>
       <c r="N25" t="n">
-        <v>3.38</v>
+        <v>3.69</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2728,15 +2728,15 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>3.49</v>
+        <v>3.61</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>15/07/2023 13:57</t>
+          <t>15/07/2023 13:58</t>
         </is>
       </c>
       <c r="R25" t="n">
-        <v>2.27</v>
+        <v>3.52</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
@@ -2744,16 +2744,16 @@
         </is>
       </c>
       <c r="T25" t="n">
-        <v>2.29</v>
+        <v>3.7</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>15/07/2023 13:57</t>
+          <t>15/07/2023 13:58</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persis-solo-borneo/d8sMcTDl/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/bali-united-madura-united/INVUe7r1/</t>
         </is>
       </c>
     </row>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -2973,14 +2973,14 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Barito Putera</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J28" t="n">
-        <v>1.6</v>
+        <v>2.97</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
@@ -2988,15 +2988,15 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>1.58</v>
+        <v>2.09</v>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>21/07/2023 09:58</t>
+          <t>21/07/2023 09:54</t>
         </is>
       </c>
       <c r="N28" t="n">
-        <v>4</v>
+        <v>3.28</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -3004,15 +3004,15 @@
         </is>
       </c>
       <c r="P28" t="n">
-        <v>4.19</v>
+        <v>3.44</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>21/07/2023 09:59</t>
+          <t>21/07/2023 09:54</t>
         </is>
       </c>
       <c r="R28" t="n">
-        <v>4.64</v>
+        <v>2.22</v>
       </c>
       <c r="S28" t="inlineStr">
         <is>
@@ -3020,16 +3020,16 @@
         </is>
       </c>
       <c r="T28" t="n">
-        <v>5.33</v>
+        <v>3.47</v>
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>21/07/2023 09:59</t>
+          <t>21/07/2023 09:54</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-ps-barito-putera/vTGPHl5K/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/pss-sleman-psis-semarang/Qme89QC0/</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -3065,14 +3065,14 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>Barito Putera</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" t="n">
-        <v>2.97</v>
+        <v>1.6</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -3080,15 +3080,15 @@
         </is>
       </c>
       <c r="L29" t="n">
-        <v>2.09</v>
+        <v>1.58</v>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>21/07/2023 09:54</t>
+          <t>21/07/2023 09:58</t>
         </is>
       </c>
       <c r="N29" t="n">
-        <v>3.28</v>
+        <v>4</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -3096,15 +3096,15 @@
         </is>
       </c>
       <c r="P29" t="n">
-        <v>3.44</v>
+        <v>4.19</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>21/07/2023 09:54</t>
+          <t>21/07/2023 09:59</t>
         </is>
       </c>
       <c r="R29" t="n">
-        <v>2.22</v>
+        <v>4.64</v>
       </c>
       <c r="S29" t="inlineStr">
         <is>
@@ -3112,16 +3112,16 @@
         </is>
       </c>
       <c r="T29" t="n">
-        <v>3.47</v>
+        <v>5.33</v>
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>21/07/2023 09:54</t>
+          <t>21/07/2023 09:59</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/pss-sleman-psis-semarang/Qme89QC0/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-ps-barito-putera/vTGPHl5K/</t>
         </is>
       </c>
     </row>
@@ -4253,22 +4253,22 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Persis Solo</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Arema FC</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
-        <v>1.65</v>
+        <v>2.32</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
@@ -4276,7 +4276,7 @@
         </is>
       </c>
       <c r="L42" t="n">
-        <v>1.61</v>
+        <v>2.79</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
@@ -4284,7 +4284,7 @@
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.8</v>
+        <v>3.26</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -4292,32 +4292,32 @@
         </is>
       </c>
       <c r="P42" t="n">
-        <v>4.15</v>
+        <v>3.5</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
+          <t>30/07/2023 09:58</t>
+        </is>
+      </c>
+      <c r="R42" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>28/07/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T42" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
           <t>30/07/2023 09:55</t>
         </is>
       </c>
-      <c r="R42" t="n">
-        <v>4.48</v>
-      </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>28/07/2023 22:12</t>
-        </is>
-      </c>
-      <c r="T42" t="n">
-        <v>5.06</v>
-      </c>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>30/07/2023 09:51</t>
-        </is>
-      </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persis-solo-arema-fc/tvOgLNBC/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-pss-sleman/pCUpNqs0/</t>
         </is>
       </c>
     </row>
@@ -4345,22 +4345,22 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persis Solo</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Arema FC</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="n">
-        <v>2.32</v>
+        <v>1.65</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -4368,7 +4368,7 @@
         </is>
       </c>
       <c r="L43" t="n">
-        <v>2.79</v>
+        <v>1.61</v>
       </c>
       <c r="M43" t="inlineStr">
         <is>
@@ -4376,7 +4376,7 @@
         </is>
       </c>
       <c r="N43" t="n">
-        <v>3.26</v>
+        <v>3.8</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -4384,15 +4384,15 @@
         </is>
       </c>
       <c r="P43" t="n">
-        <v>3.5</v>
+        <v>4.15</v>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>30/07/2023 09:58</t>
+          <t>30/07/2023 09:55</t>
         </is>
       </c>
       <c r="R43" t="n">
-        <v>2.75</v>
+        <v>4.48</v>
       </c>
       <c r="S43" t="inlineStr">
         <is>
@@ -4400,16 +4400,16 @@
         </is>
       </c>
       <c r="T43" t="n">
-        <v>2.42</v>
+        <v>5.06</v>
       </c>
       <c r="U43" t="inlineStr">
         <is>
-          <t>30/07/2023 09:55</t>
+          <t>30/07/2023 09:51</t>
         </is>
       </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-pss-sleman/pCUpNqs0/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persis-solo-arema-fc/tvOgLNBC/</t>
         </is>
       </c>
     </row>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Barito Putera</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -4445,14 +4445,14 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Madura United</t>
+          <t>Persebaya</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
-        <v>2.12</v>
+        <v>1.62</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
@@ -4460,15 +4460,15 @@
         </is>
       </c>
       <c r="L44" t="n">
-        <v>2.34</v>
+        <v>1.67</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>30/07/2023 13:51</t>
+          <t>30/07/2023 13:52</t>
         </is>
       </c>
       <c r="N44" t="n">
-        <v>3.31</v>
+        <v>3.93</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -4476,15 +4476,15 @@
         </is>
       </c>
       <c r="P44" t="n">
-        <v>3.44</v>
+        <v>3.9</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>30/07/2023 13:51</t>
+          <t>30/07/2023 13:52</t>
         </is>
       </c>
       <c r="R44" t="n">
-        <v>3.13</v>
+        <v>4.54</v>
       </c>
       <c r="S44" t="inlineStr">
         <is>
@@ -4492,16 +4492,16 @@
         </is>
       </c>
       <c r="T44" t="n">
-        <v>2.94</v>
+        <v>4.97</v>
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>30/07/2023 13:51</t>
+          <t>30/07/2023 13:52</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-madura-united/z1NcKsRI/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persija-jakarta-persebaya/2mPkM3d6/</t>
         </is>
       </c>
     </row>
@@ -4529,7 +4529,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>Barito Putera</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -4537,14 +4537,14 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Persebaya</t>
+          <t>Madura United</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J45" t="n">
-        <v>1.62</v>
+        <v>2.12</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
@@ -4552,15 +4552,15 @@
         </is>
       </c>
       <c r="L45" t="n">
-        <v>1.67</v>
+        <v>2.34</v>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>30/07/2023 13:52</t>
+          <t>30/07/2023 13:51</t>
         </is>
       </c>
       <c r="N45" t="n">
-        <v>3.93</v>
+        <v>3.31</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -4568,15 +4568,15 @@
         </is>
       </c>
       <c r="P45" t="n">
-        <v>3.9</v>
+        <v>3.44</v>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>30/07/2023 13:52</t>
+          <t>30/07/2023 13:51</t>
         </is>
       </c>
       <c r="R45" t="n">
-        <v>4.54</v>
+        <v>3.13</v>
       </c>
       <c r="S45" t="inlineStr">
         <is>
@@ -4584,16 +4584,16 @@
         </is>
       </c>
       <c r="T45" t="n">
-        <v>4.97</v>
+        <v>2.94</v>
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>30/07/2023 13:52</t>
+          <t>30/07/2023 13:51</t>
         </is>
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persija-jakarta-persebaya/2mPkM3d6/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-madura-united/z1NcKsRI/</t>
         </is>
       </c>
     </row>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Persib Bandung</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -4721,14 +4721,14 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Bali United</t>
+          <t>FC Bhayangkara</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" t="n">
-        <v>1.96</v>
+        <v>2.14</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -4736,15 +4736,15 @@
         </is>
       </c>
       <c r="L47" t="n">
-        <v>2.22</v>
+        <v>1.65</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>03/08/2023 13:58</t>
+          <t>03/08/2023 13:51</t>
         </is>
       </c>
       <c r="N47" t="n">
-        <v>3.61</v>
+        <v>3.31</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -4752,15 +4752,15 @@
         </is>
       </c>
       <c r="P47" t="n">
-        <v>3.61</v>
+        <v>4.02</v>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>03/08/2023 13:58</t>
+          <t>03/08/2023 13:51</t>
         </is>
       </c>
       <c r="R47" t="n">
-        <v>3.17</v>
+        <v>3.11</v>
       </c>
       <c r="S47" t="inlineStr">
         <is>
@@ -4768,16 +4768,16 @@
         </is>
       </c>
       <c r="T47" t="n">
-        <v>3.04</v>
+        <v>4.94</v>
       </c>
       <c r="U47" t="inlineStr">
         <is>
-          <t>03/08/2023 13:58</t>
+          <t>03/08/2023 13:51</t>
         </is>
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persib-bandung-bali-united/SYEBAREi/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-fc-bhayangkara/lrG7B7ao/</t>
         </is>
       </c>
     </row>
@@ -4805,7 +4805,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>Persib Bandung</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -4813,14 +4813,14 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>FC Bhayangkara</t>
+          <t>Bali United</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>2.14</v>
+        <v>1.96</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
@@ -4828,15 +4828,15 @@
         </is>
       </c>
       <c r="L48" t="n">
-        <v>1.65</v>
+        <v>2.22</v>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>03/08/2023 13:51</t>
+          <t>03/08/2023 13:58</t>
         </is>
       </c>
       <c r="N48" t="n">
-        <v>3.31</v>
+        <v>3.61</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4844,15 +4844,15 @@
         </is>
       </c>
       <c r="P48" t="n">
-        <v>4.02</v>
+        <v>3.61</v>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>03/08/2023 13:51</t>
+          <t>03/08/2023 13:58</t>
         </is>
       </c>
       <c r="R48" t="n">
-        <v>3.11</v>
+        <v>3.17</v>
       </c>
       <c r="S48" t="inlineStr">
         <is>
@@ -4860,16 +4860,16 @@
         </is>
       </c>
       <c r="T48" t="n">
-        <v>4.94</v>
+        <v>3.04</v>
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>03/08/2023 13:51</t>
+          <t>03/08/2023 13:58</t>
         </is>
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-fc-bhayangkara/lrG7B7ao/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persib-bandung-bali-united/SYEBAREi/</t>
         </is>
       </c>
     </row>
@@ -5081,7 +5081,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -5089,14 +5089,14 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J51" t="n">
-        <v>3.91</v>
+        <v>1.39</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
@@ -5104,15 +5104,15 @@
         </is>
       </c>
       <c r="L51" t="n">
-        <v>3.19</v>
+        <v>1.52</v>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>04/08/2023 13:55</t>
+          <t>04/08/2023 13:56</t>
         </is>
       </c>
       <c r="N51" t="n">
-        <v>3.52</v>
+        <v>4.98</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -5120,15 +5120,15 @@
         </is>
       </c>
       <c r="P51" t="n">
-        <v>2.99</v>
+        <v>4.68</v>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>04/08/2023 13:50</t>
+          <t>04/08/2023 13:56</t>
         </is>
       </c>
       <c r="R51" t="n">
-        <v>1.81</v>
+        <v>5.82</v>
       </c>
       <c r="S51" t="inlineStr">
         <is>
@@ -5136,16 +5136,16 @@
         </is>
       </c>
       <c r="T51" t="n">
-        <v>2.44</v>
+        <v>5.33</v>
       </c>
       <c r="U51" t="inlineStr">
         <is>
-          <t>04/08/2023 13:55</t>
+          <t>04/08/2023 13:56</t>
         </is>
       </c>
       <c r="V51" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/pss-sleman-persija-jakarta/zaIJ85q4/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-rans-nusantara/WQBS6qEG/</t>
         </is>
       </c>
     </row>
@@ -5173,7 +5173,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="G52" t="n">
@@ -5181,14 +5181,14 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J52" t="n">
-        <v>1.39</v>
+        <v>3.91</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -5196,15 +5196,15 @@
         </is>
       </c>
       <c r="L52" t="n">
-        <v>1.52</v>
+        <v>3.19</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>04/08/2023 13:56</t>
+          <t>04/08/2023 13:55</t>
         </is>
       </c>
       <c r="N52" t="n">
-        <v>4.98</v>
+        <v>3.52</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -5212,15 +5212,15 @@
         </is>
       </c>
       <c r="P52" t="n">
-        <v>4.68</v>
+        <v>2.99</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>04/08/2023 13:56</t>
+          <t>04/08/2023 13:50</t>
         </is>
       </c>
       <c r="R52" t="n">
-        <v>5.82</v>
+        <v>1.81</v>
       </c>
       <c r="S52" t="inlineStr">
         <is>
@@ -5228,16 +5228,16 @@
         </is>
       </c>
       <c r="T52" t="n">
-        <v>5.33</v>
+        <v>2.44</v>
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>04/08/2023 13:56</t>
+          <t>04/08/2023 13:55</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-rans-nusantara/WQBS6qEG/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/pss-sleman-persija-jakarta/zaIJ85q4/</t>
         </is>
       </c>
     </row>
@@ -5633,71 +5633,71 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>FC Bhayangkara</t>
         </is>
       </c>
       <c r="G57" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Persebaya</t>
+        </is>
+      </c>
+      <c r="I57" t="n">
         <v>2</v>
       </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>PSS Sleman</t>
-        </is>
-      </c>
-      <c r="I57" t="n">
+      <c r="J57" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>06/08/2023 22:12</t>
+        </is>
+      </c>
+      <c r="L57" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>08/08/2023 09:59</t>
+        </is>
+      </c>
+      <c r="N57" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>06/08/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P57" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>08/08/2023 09:51</t>
+        </is>
+      </c>
+      <c r="R57" t="n">
         <v>3</v>
       </c>
-      <c r="J57" t="n">
-        <v>2.04</v>
-      </c>
-      <c r="K57" t="inlineStr">
+      <c r="S57" t="inlineStr">
         <is>
           <t>06/08/2023 22:12</t>
         </is>
       </c>
-      <c r="L57" t="n">
-        <v>2.28</v>
-      </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>08/08/2023 09:56</t>
-        </is>
-      </c>
-      <c r="N57" t="n">
-        <v>3.37</v>
-      </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>06/08/2023 22:12</t>
-        </is>
-      </c>
-      <c r="P57" t="n">
-        <v>3.35</v>
-      </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>08/08/2023 09:56</t>
-        </is>
-      </c>
-      <c r="R57" t="n">
-        <v>3.29</v>
-      </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>06/08/2023 22:12</t>
-        </is>
-      </c>
       <c r="T57" t="n">
-        <v>3.13</v>
+        <v>2.99</v>
       </c>
       <c r="U57" t="inlineStr">
         <is>
-          <t>08/08/2023 09:56</t>
+          <t>08/08/2023 09:59</t>
         </is>
       </c>
       <c r="V57" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-pss-sleman/E55oN4bc/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-persebaya/021sOpqi/</t>
         </is>
       </c>
     </row>
@@ -5725,22 +5725,22 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>FC Bhayangkara</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Persebaya</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I58" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J58" t="n">
-        <v>2.15</v>
+        <v>2.04</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
@@ -5748,15 +5748,15 @@
         </is>
       </c>
       <c r="L58" t="n">
-        <v>2.3</v>
+        <v>2.28</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>08/08/2023 09:59</t>
+          <t>08/08/2023 09:56</t>
         </is>
       </c>
       <c r="N58" t="n">
-        <v>3.42</v>
+        <v>3.37</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -5764,15 +5764,15 @@
         </is>
       </c>
       <c r="P58" t="n">
-        <v>3.48</v>
+        <v>3.35</v>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>08/08/2023 09:51</t>
+          <t>08/08/2023 09:56</t>
         </is>
       </c>
       <c r="R58" t="n">
-        <v>3</v>
+        <v>3.29</v>
       </c>
       <c r="S58" t="inlineStr">
         <is>
@@ -5780,16 +5780,16 @@
         </is>
       </c>
       <c r="T58" t="n">
-        <v>2.99</v>
+        <v>3.13</v>
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>08/08/2023 09:59</t>
+          <t>08/08/2023 09:56</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-persebaya/021sOpqi/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-pss-sleman/E55oN4bc/</t>
         </is>
       </c>
     </row>
@@ -5909,7 +5909,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>Barito Putera</t>
         </is>
       </c>
       <c r="G60" t="n">
@@ -5917,14 +5917,14 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Arema FC</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="I60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J60" t="n">
-        <v>1.67</v>
+        <v>2.05</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -5932,7 +5932,7 @@
         </is>
       </c>
       <c r="L60" t="n">
-        <v>1.92</v>
+        <v>2.09</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
@@ -5940,7 +5940,7 @@
         </is>
       </c>
       <c r="N60" t="n">
-        <v>3.71</v>
+        <v>3.49</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -5948,32 +5948,32 @@
         </is>
       </c>
       <c r="P60" t="n">
-        <v>3.44</v>
+        <v>3.55</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
+          <t>09/08/2023 09:57</t>
+        </is>
+      </c>
+      <c r="R60" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>07/08/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T60" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
           <t>09/08/2023 09:59</t>
         </is>
       </c>
-      <c r="R60" t="n">
-        <v>4.45</v>
-      </c>
-      <c r="S60" t="inlineStr">
-        <is>
-          <t>07/08/2023 22:12</t>
-        </is>
-      </c>
-      <c r="T60" t="n">
-        <v>4.07</v>
-      </c>
-      <c r="U60" t="inlineStr">
-        <is>
-          <t>09/08/2023 09:58</t>
-        </is>
-      </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/psis-semarang-arema-fc/4fbbK2rG/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-dewa-united/zLgfLrT9/</t>
         </is>
       </c>
     </row>
@@ -6001,7 +6001,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Barito Putera</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="G61" t="n">
@@ -6009,14 +6009,14 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>Arema FC</t>
         </is>
       </c>
       <c r="I61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" t="n">
-        <v>2.05</v>
+        <v>1.67</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
@@ -6024,7 +6024,7 @@
         </is>
       </c>
       <c r="L61" t="n">
-        <v>2.09</v>
+        <v>1.92</v>
       </c>
       <c r="M61" t="inlineStr">
         <is>
@@ -6032,7 +6032,7 @@
         </is>
       </c>
       <c r="N61" t="n">
-        <v>3.49</v>
+        <v>3.71</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -6040,15 +6040,15 @@
         </is>
       </c>
       <c r="P61" t="n">
-        <v>3.55</v>
+        <v>3.44</v>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>09/08/2023 09:57</t>
+          <t>09/08/2023 09:59</t>
         </is>
       </c>
       <c r="R61" t="n">
-        <v>3.16</v>
+        <v>4.45</v>
       </c>
       <c r="S61" t="inlineStr">
         <is>
@@ -6056,16 +6056,16 @@
         </is>
       </c>
       <c r="T61" t="n">
-        <v>3.36</v>
+        <v>4.07</v>
       </c>
       <c r="U61" t="inlineStr">
         <is>
-          <t>09/08/2023 09:59</t>
+          <t>09/08/2023 09:58</t>
         </is>
       </c>
       <c r="V61" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-dewa-united/zLgfLrT9/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/psis-semarang-arema-fc/4fbbK2rG/</t>
         </is>
       </c>
     </row>
@@ -6093,22 +6093,22 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Madura United</t>
         </is>
       </c>
       <c r="I62" t="n">
         <v>1</v>
       </c>
       <c r="J62" t="n">
-        <v>2.01</v>
+        <v>2.35</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
@@ -6116,15 +6116,15 @@
         </is>
       </c>
       <c r="L62" t="n">
-        <v>1.94</v>
+        <v>3.19</v>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>09/08/2023 13:50</t>
+          <t>09/08/2023 13:59</t>
         </is>
       </c>
       <c r="N62" t="n">
-        <v>3.52</v>
+        <v>3.53</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -6132,32 +6132,32 @@
         </is>
       </c>
       <c r="P62" t="n">
-        <v>3.12</v>
+        <v>3.24</v>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
+          <t>09/08/2023 13:55</t>
+        </is>
+      </c>
+      <c r="R62" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>08/08/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T62" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
           <t>09/08/2023 13:59</t>
         </is>
       </c>
-      <c r="R62" t="n">
-        <v>3.21</v>
-      </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>08/08/2023 02:12</t>
-        </is>
-      </c>
-      <c r="T62" t="n">
-        <v>4.49</v>
-      </c>
-      <c r="U62" t="inlineStr">
-        <is>
-          <t>09/08/2023 13:59</t>
-        </is>
-      </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persija-jakarta-borneo/roc2JMcM/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-madura-united/Q9n7ItDS/</t>
         </is>
       </c>
     </row>
@@ -6185,22 +6185,22 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Madura United</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="I63" t="n">
         <v>1</v>
       </c>
       <c r="J63" t="n">
-        <v>2.35</v>
+        <v>2.01</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
@@ -6208,39 +6208,39 @@
         </is>
       </c>
       <c r="L63" t="n">
-        <v>3.19</v>
+        <v>1.94</v>
       </c>
       <c r="M63" t="inlineStr">
         <is>
+          <t>09/08/2023 13:50</t>
+        </is>
+      </c>
+      <c r="N63" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>08/08/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P63" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
           <t>09/08/2023 13:59</t>
         </is>
       </c>
-      <c r="N63" t="n">
-        <v>3.53</v>
-      </c>
-      <c r="O63" t="inlineStr">
+      <c r="R63" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="S63" t="inlineStr">
         <is>
           <t>08/08/2023 02:12</t>
         </is>
       </c>
-      <c r="P63" t="n">
-        <v>3.24</v>
-      </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>09/08/2023 13:55</t>
-        </is>
-      </c>
-      <c r="R63" t="n">
-        <v>2.62</v>
-      </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>08/08/2023 02:12</t>
-        </is>
-      </c>
       <c r="T63" t="n">
-        <v>2.3</v>
+        <v>4.49</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
@@ -6249,7 +6249,7 @@
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-madura-united/Q9n7ItDS/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persija-jakarta-borneo/roc2JMcM/</t>
         </is>
       </c>
     </row>
@@ -7197,22 +7197,22 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>FC Bhayangkara</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J74" t="n">
-        <v>2.81</v>
+        <v>1.75</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
@@ -7220,15 +7220,15 @@
         </is>
       </c>
       <c r="L74" t="n">
-        <v>3.19</v>
+        <v>1.91</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>18/08/2023 13:59</t>
+          <t>18/08/2023 13:51</t>
         </is>
       </c>
       <c r="N74" t="n">
-        <v>3.28</v>
+        <v>3.54</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -7236,15 +7236,15 @@
         </is>
       </c>
       <c r="P74" t="n">
-        <v>3.29</v>
+        <v>3.35</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>18/08/2023 13:59</t>
+          <t>18/08/2023 13:51</t>
         </is>
       </c>
       <c r="R74" t="n">
-        <v>2.32</v>
+        <v>4.19</v>
       </c>
       <c r="S74" t="inlineStr">
         <is>
@@ -7252,16 +7252,16 @@
         </is>
       </c>
       <c r="T74" t="n">
-        <v>2.28</v>
+        <v>4.25</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>18/08/2023 13:59</t>
+          <t>18/08/2023 13:51</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-borneo/dC1KPcKe/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-pss-sleman/EmCFQw5k/</t>
         </is>
       </c>
     </row>
@@ -7289,22 +7289,22 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>FC Bhayangkara</t>
         </is>
       </c>
       <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Borneo</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
         <v>2</v>
       </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>PSS Sleman</t>
-        </is>
-      </c>
-      <c r="I75" t="n">
-        <v>3</v>
-      </c>
       <c r="J75" t="n">
-        <v>1.75</v>
+        <v>2.81</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
@@ -7312,15 +7312,15 @@
         </is>
       </c>
       <c r="L75" t="n">
-        <v>1.91</v>
+        <v>3.19</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>18/08/2023 13:51</t>
+          <t>18/08/2023 13:59</t>
         </is>
       </c>
       <c r="N75" t="n">
-        <v>3.54</v>
+        <v>3.28</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -7328,15 +7328,15 @@
         </is>
       </c>
       <c r="P75" t="n">
-        <v>3.35</v>
+        <v>3.29</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>18/08/2023 13:51</t>
+          <t>18/08/2023 13:59</t>
         </is>
       </c>
       <c r="R75" t="n">
-        <v>4.19</v>
+        <v>2.32</v>
       </c>
       <c r="S75" t="inlineStr">
         <is>
@@ -7344,16 +7344,16 @@
         </is>
       </c>
       <c r="T75" t="n">
-        <v>4.25</v>
+        <v>2.28</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>18/08/2023 13:51</t>
+          <t>18/08/2023 13:59</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-pss-sleman/EmCFQw5k/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-borneo/dC1KPcKe/</t>
         </is>
       </c>
     </row>
@@ -7381,7 +7381,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G76" t="n">
@@ -7389,14 +7389,14 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Madura United</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="I76" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J76" t="n">
-        <v>2.79</v>
+        <v>2.38</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
@@ -7404,11 +7404,11 @@
         </is>
       </c>
       <c r="L76" t="n">
-        <v>2.94</v>
+        <v>2.33</v>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>19/08/2023 09:55</t>
+          <t>19/08/2023 09:51</t>
         </is>
       </c>
       <c r="N76" t="n">
@@ -7420,7 +7420,7 @@
         </is>
       </c>
       <c r="P76" t="n">
-        <v>3.38</v>
+        <v>3.29</v>
       </c>
       <c r="Q76" t="inlineStr">
         <is>
@@ -7428,7 +7428,7 @@
         </is>
       </c>
       <c r="R76" t="n">
-        <v>2.32</v>
+        <v>2.71</v>
       </c>
       <c r="S76" t="inlineStr">
         <is>
@@ -7436,7 +7436,7 @@
         </is>
       </c>
       <c r="T76" t="n">
-        <v>2.37</v>
+        <v>3.08</v>
       </c>
       <c r="U76" t="inlineStr">
         <is>
@@ -7445,7 +7445,7 @@
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-madura-united/zcDBRJkq/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-dewa-united/AF5OOHZ1/</t>
         </is>
       </c>
     </row>
@@ -7473,7 +7473,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G77" t="n">
@@ -7481,14 +7481,14 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>Madura United</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J77" t="n">
-        <v>2.38</v>
+        <v>2.79</v>
       </c>
       <c r="K77" t="inlineStr">
         <is>
@@ -7496,11 +7496,11 @@
         </is>
       </c>
       <c r="L77" t="n">
-        <v>2.33</v>
+        <v>2.94</v>
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>19/08/2023 09:51</t>
+          <t>19/08/2023 09:55</t>
         </is>
       </c>
       <c r="N77" t="n">
@@ -7512,7 +7512,7 @@
         </is>
       </c>
       <c r="P77" t="n">
-        <v>3.29</v>
+        <v>3.38</v>
       </c>
       <c r="Q77" t="inlineStr">
         <is>
@@ -7520,7 +7520,7 @@
         </is>
       </c>
       <c r="R77" t="n">
-        <v>2.71</v>
+        <v>2.32</v>
       </c>
       <c r="S77" t="inlineStr">
         <is>
@@ -7528,7 +7528,7 @@
         </is>
       </c>
       <c r="T77" t="n">
-        <v>3.08</v>
+        <v>2.37</v>
       </c>
       <c r="U77" t="inlineStr">
         <is>
@@ -7537,7 +7537,7 @@
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-dewa-united/AF5OOHZ1/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-madura-united/zcDBRJkq/</t>
         </is>
       </c>
     </row>
@@ -7933,22 +7933,22 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Persik Kediri</t>
+          <t>Madura United</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>FC Bhayangkara</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J82" t="n">
-        <v>2.11</v>
+        <v>1.76</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -7956,15 +7956,15 @@
         </is>
       </c>
       <c r="L82" t="n">
-        <v>1.86</v>
+        <v>1.59</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>25/08/2023 09:58</t>
+          <t>25/08/2023 09:55</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>3.28</v>
+        <v>3.57</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -7972,15 +7972,15 @@
         </is>
       </c>
       <c r="P82" t="n">
-        <v>3.69</v>
+        <v>4</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>25/08/2023 09:58</t>
+          <t>25/08/2023 09:55</t>
         </is>
       </c>
       <c r="R82" t="n">
-        <v>3.11</v>
+        <v>3.95</v>
       </c>
       <c r="S82" t="inlineStr">
         <is>
@@ -7988,16 +7988,16 @@
         </is>
       </c>
       <c r="T82" t="n">
-        <v>4.02</v>
+        <v>5.59</v>
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>25/08/2023 09:58</t>
+          <t>25/08/2023 09:55</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-psis-semarang/SjxkuwKr/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/madura-united-fc-bhayangkara/AFRgvcZl/</t>
         </is>
       </c>
     </row>
@@ -8025,22 +8025,22 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Madura United</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>FC Bhayangkara</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>1.76</v>
+        <v>2.11</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -8048,15 +8048,15 @@
         </is>
       </c>
       <c r="L83" t="n">
-        <v>1.59</v>
+        <v>1.86</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>25/08/2023 09:55</t>
+          <t>25/08/2023 09:58</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>3.57</v>
+        <v>3.28</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -8064,15 +8064,15 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>4</v>
+        <v>3.69</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>25/08/2023 09:55</t>
+          <t>25/08/2023 09:58</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>3.95</v>
+        <v>3.11</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
@@ -8080,16 +8080,16 @@
         </is>
       </c>
       <c r="T83" t="n">
-        <v>5.59</v>
+        <v>4.02</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>25/08/2023 09:55</t>
+          <t>25/08/2023 09:58</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/madura-united-fc-bhayangkara/AFRgvcZl/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-psis-semarang/SjxkuwKr/</t>
         </is>
       </c>
     </row>
@@ -8117,7 +8117,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -8125,14 +8125,14 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.85</v>
+        <v>3.11</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -8140,15 +8140,15 @@
         </is>
       </c>
       <c r="L84" t="n">
-        <v>1.64</v>
+        <v>2.6</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>25/08/2023 13:51</t>
+          <t>25/08/2023 13:59</t>
         </is>
       </c>
       <c r="N84" t="n">
-        <v>3.73</v>
+        <v>3.17</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -8156,15 +8156,15 @@
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.9</v>
+        <v>3.11</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>25/08/2023 13:51</t>
+          <t>25/08/2023 13:59</t>
         </is>
       </c>
       <c r="R84" t="n">
-        <v>3.51</v>
+        <v>2.15</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
@@ -8172,16 +8172,16 @@
         </is>
       </c>
       <c r="T84" t="n">
-        <v>5.27</v>
+        <v>2.84</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>25/08/2023 13:51</t>
+          <t>25/08/2023 13:59</t>
         </is>
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-persita/l6QcwHle/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/dewa-united-persija-jakarta/IuV1xy41/</t>
         </is>
       </c>
     </row>
@@ -8209,7 +8209,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="G85" t="n">
@@ -8217,14 +8217,14 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J85" t="n">
-        <v>3.11</v>
+        <v>1.85</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -8232,15 +8232,15 @@
         </is>
       </c>
       <c r="L85" t="n">
-        <v>2.6</v>
+        <v>1.64</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>25/08/2023 13:59</t>
+          <t>25/08/2023 13:51</t>
         </is>
       </c>
       <c r="N85" t="n">
-        <v>3.17</v>
+        <v>3.73</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -8248,15 +8248,15 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.11</v>
+        <v>3.9</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>25/08/2023 13:59</t>
+          <t>25/08/2023 13:51</t>
         </is>
       </c>
       <c r="R85" t="n">
-        <v>2.15</v>
+        <v>3.51</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
@@ -8264,16 +8264,16 @@
         </is>
       </c>
       <c r="T85" t="n">
-        <v>2.84</v>
+        <v>5.27</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>25/08/2023 13:59</t>
+          <t>25/08/2023 13:51</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/dewa-united-persija-jakarta/IuV1xy41/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-persita/l6QcwHle/</t>
         </is>
       </c>
     </row>
@@ -9221,71 +9221,71 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>Persebaya</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.6</v>
+        <v>2.49</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>01/09/2023 22:12</t>
+          <t>01/09/2023 22:13</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>4.06</v>
+        <v>2.74</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>03/09/2023 09:13</t>
+          <t>03/09/2023 09:59</t>
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.1</v>
+        <v>3.11</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>01/09/2023 22:12</t>
+          <t>01/09/2023 22:13</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.54</v>
+        <v>3.26</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>03/09/2023 09:19</t>
+          <t>03/09/2023 09:58</t>
         </is>
       </c>
       <c r="R96" t="n">
-        <v>2.51</v>
+        <v>2.71</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
-          <t>01/09/2023 22:12</t>
+          <t>01/09/2023 22:13</t>
         </is>
       </c>
       <c r="T96" t="n">
-        <v>1.89</v>
+        <v>2.59</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>03/09/2023 09:19</t>
+          <t>03/09/2023 09:59</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-dewa-united/lv4QvUPa/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persebaya-borneo/j7Qef9Pn/</t>
         </is>
       </c>
     </row>
@@ -9313,71 +9313,71 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Persebaya</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.49</v>
+        <v>2.6</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>01/09/2023 22:13</t>
+          <t>01/09/2023 22:12</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>2.74</v>
+        <v>4.06</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>03/09/2023 09:59</t>
+          <t>03/09/2023 09:13</t>
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.11</v>
+        <v>3.1</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>01/09/2023 22:13</t>
+          <t>01/09/2023 22:12</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3.26</v>
+        <v>3.54</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
-          <t>03/09/2023 09:58</t>
+          <t>03/09/2023 09:19</t>
         </is>
       </c>
       <c r="R97" t="n">
-        <v>2.71</v>
+        <v>2.51</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
-          <t>01/09/2023 22:13</t>
+          <t>01/09/2023 22:12</t>
         </is>
       </c>
       <c r="T97" t="n">
-        <v>2.59</v>
+        <v>1.89</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
-          <t>03/09/2023 09:59</t>
+          <t>03/09/2023 09:19</t>
         </is>
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persebaya-borneo/j7Qef9Pn/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-dewa-united/lv4QvUPa/</t>
         </is>
       </c>
     </row>
@@ -12073,7 +12073,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G127" t="n">
@@ -12081,11 +12081,11 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Persis Solo</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="I127" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J127" t="n">
         <v>2.54</v>
@@ -12096,15 +12096,15 @@
         </is>
       </c>
       <c r="L127" t="n">
-        <v>3.74</v>
+        <v>3.07</v>
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>06/10/2023 09:56</t>
+          <t>06/10/2023 09:52</t>
         </is>
       </c>
       <c r="N127" t="n">
-        <v>3.24</v>
+        <v>3.19</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -12112,15 +12112,15 @@
         </is>
       </c>
       <c r="P127" t="n">
-        <v>3.73</v>
+        <v>3.19</v>
       </c>
       <c r="Q127" t="inlineStr">
         <is>
-          <t>06/10/2023 09:58</t>
+          <t>06/10/2023 09:52</t>
         </is>
       </c>
       <c r="R127" t="n">
-        <v>2.52</v>
+        <v>2.54</v>
       </c>
       <c r="S127" t="inlineStr">
         <is>
@@ -12128,16 +12128,16 @@
         </is>
       </c>
       <c r="T127" t="n">
-        <v>1.92</v>
+        <v>2.39</v>
       </c>
       <c r="U127" t="inlineStr">
         <is>
-          <t>06/10/2023 09:56</t>
+          <t>06/10/2023 09:52</t>
         </is>
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-persis-solo/OE3fW2x4/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-psis-semarang/j15nYO7i/</t>
         </is>
       </c>
     </row>
@@ -12165,7 +12165,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G128" t="n">
@@ -12173,11 +12173,11 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>Persis Solo</t>
         </is>
       </c>
       <c r="I128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J128" t="n">
         <v>2.54</v>
@@ -12188,15 +12188,15 @@
         </is>
       </c>
       <c r="L128" t="n">
-        <v>3.07</v>
+        <v>3.74</v>
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>06/10/2023 09:52</t>
+          <t>06/10/2023 09:56</t>
         </is>
       </c>
       <c r="N128" t="n">
-        <v>3.19</v>
+        <v>3.24</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -12204,15 +12204,15 @@
         </is>
       </c>
       <c r="P128" t="n">
-        <v>3.19</v>
+        <v>3.73</v>
       </c>
       <c r="Q128" t="inlineStr">
         <is>
-          <t>06/10/2023 09:52</t>
+          <t>06/10/2023 09:58</t>
         </is>
       </c>
       <c r="R128" t="n">
-        <v>2.54</v>
+        <v>2.52</v>
       </c>
       <c r="S128" t="inlineStr">
         <is>
@@ -12220,16 +12220,16 @@
         </is>
       </c>
       <c r="T128" t="n">
-        <v>2.39</v>
+        <v>1.92</v>
       </c>
       <c r="U128" t="inlineStr">
         <is>
-          <t>06/10/2023 09:52</t>
+          <t>06/10/2023 09:56</t>
         </is>
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-psis-semarang/j15nYO7i/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-persis-solo/OE3fW2x4/</t>
         </is>
       </c>
     </row>
@@ -12901,71 +12901,71 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Bali United</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G136" t="n">
+        <v>2</v>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>PSIS Semarang</t>
+        </is>
+      </c>
+      <c r="I136" t="n">
         <v>3</v>
       </c>
-      <c r="H136" t="inlineStr">
-        <is>
-          <t>Persebaya</t>
-        </is>
-      </c>
-      <c r="I136" t="n">
-        <v>1</v>
-      </c>
       <c r="J136" t="n">
+        <v>2.99</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>18/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L136" t="n">
+        <v>3.66</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>20/10/2023 09:49</t>
+        </is>
+      </c>
+      <c r="N136" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>18/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P136" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>20/10/2023 09:49</t>
+        </is>
+      </c>
+      <c r="R136" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>18/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T136" t="n">
         <v>1.89</v>
       </c>
-      <c r="K136" t="inlineStr">
-        <is>
-          <t>18/10/2023 21:12</t>
-        </is>
-      </c>
-      <c r="L136" t="n">
-        <v>1.76</v>
-      </c>
-      <c r="M136" t="inlineStr">
-        <is>
-          <t>20/10/2023 09:57</t>
-        </is>
-      </c>
-      <c r="N136" t="n">
-        <v>3.54</v>
-      </c>
-      <c r="O136" t="inlineStr">
-        <is>
-          <t>18/10/2023 21:12</t>
-        </is>
-      </c>
-      <c r="P136" t="n">
-        <v>3.84</v>
-      </c>
-      <c r="Q136" t="inlineStr">
-        <is>
-          <t>20/10/2023 09:57</t>
-        </is>
-      </c>
-      <c r="R136" t="n">
-        <v>3.43</v>
-      </c>
-      <c r="S136" t="inlineStr">
-        <is>
-          <t>18/10/2023 21:12</t>
-        </is>
-      </c>
-      <c r="T136" t="n">
-        <v>4.38</v>
-      </c>
       <c r="U136" t="inlineStr">
         <is>
-          <t>20/10/2023 09:57</t>
+          <t>20/10/2023 09:49</t>
         </is>
       </c>
       <c r="V136" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/bali-united-persebaya/jP3ZWZSE/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-psis-semarang/CY4VXFD8/</t>
         </is>
       </c>
     </row>
@@ -12993,22 +12993,22 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>Bali United</t>
         </is>
       </c>
       <c r="G137" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>Persebaya</t>
         </is>
       </c>
       <c r="I137" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J137" t="n">
-        <v>2.99</v>
+        <v>1.89</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
@@ -13016,15 +13016,15 @@
         </is>
       </c>
       <c r="L137" t="n">
-        <v>3.66</v>
+        <v>1.76</v>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>20/10/2023 09:49</t>
+          <t>20/10/2023 09:57</t>
         </is>
       </c>
       <c r="N137" t="n">
-        <v>3.24</v>
+        <v>3.54</v>
       </c>
       <c r="O137" t="inlineStr">
         <is>
@@ -13032,15 +13032,15 @@
         </is>
       </c>
       <c r="P137" t="n">
-        <v>3.27</v>
+        <v>3.84</v>
       </c>
       <c r="Q137" t="inlineStr">
         <is>
-          <t>20/10/2023 09:49</t>
+          <t>20/10/2023 09:57</t>
         </is>
       </c>
       <c r="R137" t="n">
-        <v>2.18</v>
+        <v>3.43</v>
       </c>
       <c r="S137" t="inlineStr">
         <is>
@@ -13048,16 +13048,16 @@
         </is>
       </c>
       <c r="T137" t="n">
-        <v>1.89</v>
+        <v>4.38</v>
       </c>
       <c r="U137" t="inlineStr">
         <is>
-          <t>20/10/2023 09:49</t>
+          <t>20/10/2023 09:57</t>
         </is>
       </c>
       <c r="V137" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-psis-semarang/CY4VXFD8/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/bali-united-persebaya/jP3ZWZSE/</t>
         </is>
       </c>
     </row>
@@ -14530,6 +14530,98 @@
       <c r="V153" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/indonesia/liga-1/bali-united-persita/AF99DTs0/</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>indonesia</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>liga-1</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E154" s="2" t="n">
+        <v>45231.54166666666</v>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Madura United</t>
+        </is>
+      </c>
+      <c r="G154" t="n">
+        <v>0</v>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>Persib Bandung</t>
+        </is>
+      </c>
+      <c r="I154" t="n">
+        <v>1</v>
+      </c>
+      <c r="J154" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L154" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="M154" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:59</t>
+        </is>
+      </c>
+      <c r="N154" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="O154" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P154" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:57</t>
+        </is>
+      </c>
+      <c r="R154" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="S154" t="inlineStr">
+        <is>
+          <t>31/10/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T154" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="U154" t="inlineStr">
+        <is>
+          <t>01/11/2023 12:33</t>
+        </is>
+      </c>
+      <c r="V154" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/madura-united-persib-bandung/GhWzUlSt/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 02-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/indonesia_liga-1_2023-2024.xlsx
+++ b/2023/indonesia_liga-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V154"/>
+  <dimension ref="A1:V155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14625,6 +14625,98 @@
         </is>
       </c>
     </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>indonesia</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>liga-1</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E155" s="2" t="n">
+        <v>45232.375</v>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Arema FC</t>
+        </is>
+      </c>
+      <c r="G155" t="n">
+        <v>2</v>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>Dewa United</t>
+        </is>
+      </c>
+      <c r="I155" t="n">
+        <v>1</v>
+      </c>
+      <c r="J155" t="n">
+        <v>2.71</v>
+      </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>31/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="L155" t="n">
+        <v>3.19</v>
+      </c>
+      <c r="M155" t="inlineStr">
+        <is>
+          <t>02/11/2023 08:59</t>
+        </is>
+      </c>
+      <c r="N155" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="O155" t="inlineStr">
+        <is>
+          <t>31/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="P155" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="Q155" t="inlineStr">
+        <is>
+          <t>02/11/2023 08:59</t>
+        </is>
+      </c>
+      <c r="R155" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="S155" t="inlineStr">
+        <is>
+          <t>31/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T155" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="U155" t="inlineStr">
+        <is>
+          <t>02/11/2023 08:58</t>
+        </is>
+      </c>
+      <c r="V155" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/arema-fc-dewa-united/4E2IB7CC/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizado por script em 08-11-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/indonesia_liga-1_2023-2024.xlsx
+++ b/2023/indonesia_liga-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V161"/>
+  <dimension ref="A1:V163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2413,22 +2413,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Persik Kediri</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Arema FC</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J22" t="n">
-        <v>1.71</v>
+        <v>2.52</v>
       </c>
       <c r="K22" t="inlineStr">
         <is>
@@ -2436,15 +2436,15 @@
         </is>
       </c>
       <c r="L22" t="n">
-        <v>2.08</v>
+        <v>2.85</v>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>15/07/2023 09:52</t>
+          <t>15/07/2023 09:59</t>
         </is>
       </c>
       <c r="N22" t="n">
-        <v>3.61</v>
+        <v>3.33</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2452,15 +2452,15 @@
         </is>
       </c>
       <c r="P22" t="n">
-        <v>3.29</v>
+        <v>3.45</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>15/07/2023 09:52</t>
+          <t>15/07/2023 09:50</t>
         </is>
       </c>
       <c r="R22" t="n">
-        <v>4.32</v>
+        <v>2.54</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
@@ -2468,16 +2468,16 @@
         </is>
       </c>
       <c r="T22" t="n">
-        <v>3.66</v>
+        <v>2.4</v>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>15/07/2023 09:52</t>
+          <t>15/07/2023 09:59</t>
         </is>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-arema-fc/vXWQdmTf/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-persita/nczZfRc7/</t>
         </is>
       </c>
     </row>
@@ -2505,22 +2505,22 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>Arema FC</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J23" t="n">
-        <v>2.52</v>
+        <v>1.71</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
@@ -2528,15 +2528,15 @@
         </is>
       </c>
       <c r="L23" t="n">
-        <v>2.85</v>
+        <v>2.08</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>15/07/2023 09:59</t>
+          <t>15/07/2023 09:52</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>3.33</v>
+        <v>3.61</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2544,15 +2544,15 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>3.45</v>
+        <v>3.29</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>15/07/2023 09:50</t>
+          <t>15/07/2023 09:52</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>2.54</v>
+        <v>4.32</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
@@ -2560,16 +2560,16 @@
         </is>
       </c>
       <c r="T23" t="n">
-        <v>2.4</v>
+        <v>3.66</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>15/07/2023 09:59</t>
+          <t>15/07/2023 09:52</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-persita/nczZfRc7/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-arema-fc/vXWQdmTf/</t>
         </is>
       </c>
     </row>
@@ -3793,22 +3793,22 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J37" t="n">
-        <v>2.69</v>
+        <v>2.25</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
@@ -3816,7 +3816,7 @@
         </is>
       </c>
       <c r="L37" t="n">
-        <v>2.35</v>
+        <v>4.33</v>
       </c>
       <c r="M37" t="inlineStr">
         <is>
@@ -3824,7 +3824,7 @@
         </is>
       </c>
       <c r="N37" t="n">
-        <v>3.32</v>
+        <v>3.15</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3832,7 +3832,7 @@
         </is>
       </c>
       <c r="P37" t="n">
-        <v>3.96</v>
+        <v>3.55</v>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
@@ -3840,7 +3840,7 @@
         </is>
       </c>
       <c r="R37" t="n">
-        <v>2.34</v>
+        <v>2.94</v>
       </c>
       <c r="S37" t="inlineStr">
         <is>
@@ -3848,7 +3848,7 @@
         </is>
       </c>
       <c r="T37" t="n">
-        <v>2.63</v>
+        <v>1.83</v>
       </c>
       <c r="U37" t="inlineStr">
         <is>
@@ -3857,7 +3857,7 @@
       </c>
       <c r="V37" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/psis-semarang-borneo/ENj2V7ZJ/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-persita/hEk6URlQ/</t>
         </is>
       </c>
     </row>
@@ -3885,22 +3885,22 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
-        <v>2.25</v>
+        <v>2.69</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
@@ -3908,7 +3908,7 @@
         </is>
       </c>
       <c r="L38" t="n">
-        <v>4.33</v>
+        <v>2.35</v>
       </c>
       <c r="M38" t="inlineStr">
         <is>
@@ -3916,7 +3916,7 @@
         </is>
       </c>
       <c r="N38" t="n">
-        <v>3.15</v>
+        <v>3.32</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3924,7 +3924,7 @@
         </is>
       </c>
       <c r="P38" t="n">
-        <v>3.55</v>
+        <v>3.96</v>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
@@ -3932,7 +3932,7 @@
         </is>
       </c>
       <c r="R38" t="n">
-        <v>2.94</v>
+        <v>2.34</v>
       </c>
       <c r="S38" t="inlineStr">
         <is>
@@ -3940,7 +3940,7 @@
         </is>
       </c>
       <c r="T38" t="n">
-        <v>1.83</v>
+        <v>2.63</v>
       </c>
       <c r="U38" t="inlineStr">
         <is>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-persita/hEk6URlQ/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/psis-semarang-borneo/ENj2V7ZJ/</t>
         </is>
       </c>
     </row>
@@ -7381,7 +7381,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G76" t="n">
@@ -7389,14 +7389,14 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Madura United</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="I76" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J76" t="n">
-        <v>2.79</v>
+        <v>2.38</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
@@ -7404,11 +7404,11 @@
         </is>
       </c>
       <c r="L76" t="n">
-        <v>2.94</v>
+        <v>2.33</v>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>19/08/2023 09:55</t>
+          <t>19/08/2023 09:51</t>
         </is>
       </c>
       <c r="N76" t="n">
@@ -7420,7 +7420,7 @@
         </is>
       </c>
       <c r="P76" t="n">
-        <v>3.38</v>
+        <v>3.29</v>
       </c>
       <c r="Q76" t="inlineStr">
         <is>
@@ -7428,7 +7428,7 @@
         </is>
       </c>
       <c r="R76" t="n">
-        <v>2.32</v>
+        <v>2.71</v>
       </c>
       <c r="S76" t="inlineStr">
         <is>
@@ -7436,7 +7436,7 @@
         </is>
       </c>
       <c r="T76" t="n">
-        <v>2.37</v>
+        <v>3.08</v>
       </c>
       <c r="U76" t="inlineStr">
         <is>
@@ -7445,7 +7445,7 @@
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-madura-united/zcDBRJkq/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-dewa-united/AF5OOHZ1/</t>
         </is>
       </c>
     </row>
@@ -7473,7 +7473,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G77" t="n">
@@ -7481,14 +7481,14 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>Madura United</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J77" t="n">
-        <v>2.38</v>
+        <v>2.79</v>
       </c>
       <c r="K77" t="inlineStr">
         <is>
@@ -7496,11 +7496,11 @@
         </is>
       </c>
       <c r="L77" t="n">
-        <v>2.33</v>
+        <v>2.94</v>
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>19/08/2023 09:51</t>
+          <t>19/08/2023 09:55</t>
         </is>
       </c>
       <c r="N77" t="n">
@@ -7512,7 +7512,7 @@
         </is>
       </c>
       <c r="P77" t="n">
-        <v>3.29</v>
+        <v>3.38</v>
       </c>
       <c r="Q77" t="inlineStr">
         <is>
@@ -7520,7 +7520,7 @@
         </is>
       </c>
       <c r="R77" t="n">
-        <v>2.71</v>
+        <v>2.32</v>
       </c>
       <c r="S77" t="inlineStr">
         <is>
@@ -7528,7 +7528,7 @@
         </is>
       </c>
       <c r="T77" t="n">
-        <v>3.08</v>
+        <v>2.37</v>
       </c>
       <c r="U77" t="inlineStr">
         <is>
@@ -7537,7 +7537,7 @@
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-dewa-united/AF5OOHZ1/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-madura-united/zcDBRJkq/</t>
         </is>
       </c>
     </row>
@@ -9221,71 +9221,71 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Persebaya</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>2.49</v>
+        <v>2.6</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>01/09/2023 22:13</t>
+          <t>01/09/2023 22:12</t>
         </is>
       </c>
       <c r="L96" t="n">
-        <v>2.74</v>
+        <v>4.06</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>03/09/2023 09:59</t>
+          <t>03/09/2023 09:13</t>
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.11</v>
+        <v>3.1</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
-          <t>01/09/2023 22:13</t>
+          <t>01/09/2023 22:12</t>
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.26</v>
+        <v>3.54</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>03/09/2023 09:58</t>
+          <t>03/09/2023 09:19</t>
         </is>
       </c>
       <c r="R96" t="n">
-        <v>2.71</v>
+        <v>2.51</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
-          <t>01/09/2023 22:13</t>
+          <t>01/09/2023 22:12</t>
         </is>
       </c>
       <c r="T96" t="n">
-        <v>2.59</v>
+        <v>1.89</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>03/09/2023 09:59</t>
+          <t>03/09/2023 09:19</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persebaya-borneo/j7Qef9Pn/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-dewa-united/lv4QvUPa/</t>
         </is>
       </c>
     </row>
@@ -9313,71 +9313,71 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>Persebaya</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>2.6</v>
+        <v>2.49</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>01/09/2023 22:12</t>
+          <t>01/09/2023 22:13</t>
         </is>
       </c>
       <c r="L97" t="n">
-        <v>4.06</v>
+        <v>2.74</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>03/09/2023 09:13</t>
+          <t>03/09/2023 09:59</t>
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.1</v>
+        <v>3.11</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
-          <t>01/09/2023 22:12</t>
+          <t>01/09/2023 22:13</t>
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3.54</v>
+        <v>3.26</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
-          <t>03/09/2023 09:19</t>
+          <t>03/09/2023 09:58</t>
         </is>
       </c>
       <c r="R97" t="n">
-        <v>2.51</v>
+        <v>2.71</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
-          <t>01/09/2023 22:12</t>
+          <t>01/09/2023 22:13</t>
         </is>
       </c>
       <c r="T97" t="n">
-        <v>1.89</v>
+        <v>2.59</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
-          <t>03/09/2023 09:19</t>
+          <t>03/09/2023 09:59</t>
         </is>
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-dewa-united/lv4QvUPa/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persebaya-borneo/j7Qef9Pn/</t>
         </is>
       </c>
     </row>
@@ -10233,7 +10233,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Persik Kediri</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -10241,14 +10241,14 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I107" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J107" t="n">
-        <v>2.82</v>
+        <v>1.56</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -10256,15 +10256,15 @@
         </is>
       </c>
       <c r="L107" t="n">
-        <v>3.07</v>
+        <v>1.5</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>17/09/2023 13:52</t>
+          <t>17/09/2023 13:53</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>3.09</v>
+        <v>4.05</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -10272,15 +10272,15 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>2.94</v>
+        <v>4.47</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>17/09/2023 13:52</t>
+          <t>17/09/2023 13:53</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>2.37</v>
+        <v>4.92</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
@@ -10288,16 +10288,16 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>2.55</v>
+        <v>6.08</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>17/09/2023 13:52</t>
+          <t>17/09/2023 13:53</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-persija-jakarta/r1kZ7Sgn/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-pss-sleman/4AjV88vt/</t>
         </is>
       </c>
     </row>
@@ -10325,7 +10325,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="G108" t="n">
@@ -10333,14 +10333,14 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="I108" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J108" t="n">
-        <v>1.56</v>
+        <v>2.82</v>
       </c>
       <c r="K108" t="inlineStr">
         <is>
@@ -10348,15 +10348,15 @@
         </is>
       </c>
       <c r="L108" t="n">
-        <v>1.5</v>
+        <v>3.07</v>
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>17/09/2023 13:53</t>
+          <t>17/09/2023 13:52</t>
         </is>
       </c>
       <c r="N108" t="n">
-        <v>4.05</v>
+        <v>3.09</v>
       </c>
       <c r="O108" t="inlineStr">
         <is>
@@ -10364,15 +10364,15 @@
         </is>
       </c>
       <c r="P108" t="n">
-        <v>4.47</v>
+        <v>2.94</v>
       </c>
       <c r="Q108" t="inlineStr">
         <is>
-          <t>17/09/2023 13:53</t>
+          <t>17/09/2023 13:52</t>
         </is>
       </c>
       <c r="R108" t="n">
-        <v>4.92</v>
+        <v>2.37</v>
       </c>
       <c r="S108" t="inlineStr">
         <is>
@@ -10380,16 +10380,16 @@
         </is>
       </c>
       <c r="T108" t="n">
-        <v>6.08</v>
+        <v>2.55</v>
       </c>
       <c r="U108" t="inlineStr">
         <is>
-          <t>17/09/2023 13:53</t>
+          <t>17/09/2023 13:52</t>
         </is>
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-pss-sleman/4AjV88vt/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-persija-jakarta/r1kZ7Sgn/</t>
         </is>
       </c>
     </row>
@@ -12257,22 +12257,22 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Arema FC</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="G129" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I129" t="n">
         <v>1</v>
       </c>
       <c r="J129" t="n">
-        <v>3.87</v>
+        <v>1.74</v>
       </c>
       <c r="K129" t="inlineStr">
         <is>
@@ -12280,15 +12280,15 @@
         </is>
       </c>
       <c r="L129" t="n">
-        <v>3.69</v>
+        <v>1.56</v>
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>06/10/2023 13:57</t>
+          <t>06/10/2023 13:43</t>
         </is>
       </c>
       <c r="N129" t="n">
-        <v>3.45</v>
+        <v>3.56</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -12296,15 +12296,15 @@
         </is>
       </c>
       <c r="P129" t="n">
-        <v>3.36</v>
+        <v>4.04</v>
       </c>
       <c r="Q129" t="inlineStr">
         <is>
-          <t>06/10/2023 13:57</t>
+          <t>06/10/2023 13:43</t>
         </is>
       </c>
       <c r="R129" t="n">
-        <v>1.81</v>
+        <v>4.07</v>
       </c>
       <c r="S129" t="inlineStr">
         <is>
@@ -12312,16 +12312,16 @@
         </is>
       </c>
       <c r="T129" t="n">
-        <v>2.04</v>
+        <v>5.98</v>
       </c>
       <c r="U129" t="inlineStr">
         <is>
-          <t>06/10/2023 13:58</t>
+          <t>06/10/2023 13:43</t>
         </is>
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/arema-fc-borneo/Ui4jXrNc/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/dewa-united-pss-sleman/xI7bVMiA/</t>
         </is>
       </c>
     </row>
@@ -12349,22 +12349,22 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>Arema FC</t>
         </is>
       </c>
       <c r="G130" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="I130" t="n">
         <v>1</v>
       </c>
       <c r="J130" t="n">
-        <v>1.74</v>
+        <v>3.87</v>
       </c>
       <c r="K130" t="inlineStr">
         <is>
@@ -12372,15 +12372,15 @@
         </is>
       </c>
       <c r="L130" t="n">
-        <v>1.56</v>
+        <v>3.69</v>
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>06/10/2023 13:43</t>
+          <t>06/10/2023 13:57</t>
         </is>
       </c>
       <c r="N130" t="n">
-        <v>3.56</v>
+        <v>3.45</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -12388,15 +12388,15 @@
         </is>
       </c>
       <c r="P130" t="n">
-        <v>4.04</v>
+        <v>3.36</v>
       </c>
       <c r="Q130" t="inlineStr">
         <is>
-          <t>06/10/2023 13:43</t>
+          <t>06/10/2023 13:57</t>
         </is>
       </c>
       <c r="R130" t="n">
-        <v>4.07</v>
+        <v>1.81</v>
       </c>
       <c r="S130" t="inlineStr">
         <is>
@@ -12404,16 +12404,16 @@
         </is>
       </c>
       <c r="T130" t="n">
-        <v>5.98</v>
+        <v>2.04</v>
       </c>
       <c r="U130" t="inlineStr">
         <is>
-          <t>06/10/2023 13:43</t>
+          <t>06/10/2023 13:58</t>
         </is>
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/dewa-united-pss-sleman/xI7bVMiA/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/arema-fc-borneo/Ui4jXrNc/</t>
         </is>
       </c>
     </row>
@@ -15266,6 +15266,190 @@
       <c r="V161" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-ps-barito-putera/OIZrSSdg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>indonesia</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>liga-1</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E162" s="2" t="n">
+        <v>45238.375</v>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Persib Bandung</t>
+        </is>
+      </c>
+      <c r="G162" t="n">
+        <v>2</v>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>Arema FC</t>
+        </is>
+      </c>
+      <c r="I162" t="n">
+        <v>2</v>
+      </c>
+      <c r="J162" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>06/11/2023 21:13</t>
+        </is>
+      </c>
+      <c r="L162" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="M162" t="inlineStr">
+        <is>
+          <t>08/11/2023 08:55</t>
+        </is>
+      </c>
+      <c r="N162" t="n">
+        <v>4.88</v>
+      </c>
+      <c r="O162" t="inlineStr">
+        <is>
+          <t>06/11/2023 21:13</t>
+        </is>
+      </c>
+      <c r="P162" t="n">
+        <v>5.42</v>
+      </c>
+      <c r="Q162" t="inlineStr">
+        <is>
+          <t>08/11/2023 08:55</t>
+        </is>
+      </c>
+      <c r="R162" t="n">
+        <v>7.04</v>
+      </c>
+      <c r="S162" t="inlineStr">
+        <is>
+          <t>06/11/2023 21:13</t>
+        </is>
+      </c>
+      <c r="T162" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="U162" t="inlineStr">
+        <is>
+          <t>08/11/2023 08:55</t>
+        </is>
+      </c>
+      <c r="V162" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persib-bandung-arema-fc/MBllPQtC/</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>indonesia</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>liga-1</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E163" s="2" t="n">
+        <v>45238.375</v>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Persik Kediri</t>
+        </is>
+      </c>
+      <c r="G163" t="n">
+        <v>4</v>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>Madura United</t>
+        </is>
+      </c>
+      <c r="I163" t="n">
+        <v>0</v>
+      </c>
+      <c r="J163" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>06/11/2023 21:11</t>
+        </is>
+      </c>
+      <c r="L163" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="M163" t="inlineStr">
+        <is>
+          <t>08/11/2023 08:47</t>
+        </is>
+      </c>
+      <c r="N163" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>06/11/2023 21:11</t>
+        </is>
+      </c>
+      <c r="P163" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>08/11/2023 08:47</t>
+        </is>
+      </c>
+      <c r="R163" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="S163" t="inlineStr">
+        <is>
+          <t>06/11/2023 21:11</t>
+        </is>
+      </c>
+      <c r="T163" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="U163" t="inlineStr">
+        <is>
+          <t>08/11/2023 08:45</t>
+        </is>
+      </c>
+      <c r="V163" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-madura-united/rLkpQ6R5/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 09-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/indonesia_liga-1_2023-2024.xlsx
+++ b/2023/indonesia_liga-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V166"/>
+  <dimension ref="A1:V168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,22 +2137,22 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>Barito Putera</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>PSM Makassar</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I19" t="n">
         <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>3.73</v>
+        <v>1.56</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
@@ -2160,15 +2160,15 @@
         </is>
       </c>
       <c r="L19" t="n">
-        <v>3.53</v>
+        <v>1.86</v>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>14/07/2023 09:53</t>
+          <t>14/07/2023 09:58</t>
         </is>
       </c>
       <c r="N19" t="n">
-        <v>3.49</v>
+        <v>4.07</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
@@ -2176,15 +2176,15 @@
         </is>
       </c>
       <c r="P19" t="n">
-        <v>3.33</v>
+        <v>3.27</v>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>14/07/2023 09:53</t>
+          <t>14/07/2023 09:57</t>
         </is>
       </c>
       <c r="R19" t="n">
-        <v>1.86</v>
+        <v>4.9</v>
       </c>
       <c r="S19" t="inlineStr">
         <is>
@@ -2192,16 +2192,16 @@
         </is>
       </c>
       <c r="T19" t="n">
-        <v>2.11</v>
+        <v>3.05</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>14/07/2023 09:53</t>
+          <t>14/07/2023 09:58</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-psm-makassar/QPjj3kjR/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-pss-sleman/nZin4VzL/</t>
         </is>
       </c>
     </row>
@@ -2229,22 +2229,22 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Barito Putera</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>PSM Makassar</t>
         </is>
       </c>
       <c r="I20" t="n">
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>1.56</v>
+        <v>3.73</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
@@ -2252,48 +2252,48 @@
         </is>
       </c>
       <c r="L20" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>14/07/2023 09:53</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>12/07/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>14/07/2023 09:53</t>
+        </is>
+      </c>
+      <c r="R20" t="n">
         <v>1.86</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>14/07/2023 09:58</t>
-        </is>
-      </c>
-      <c r="N20" t="n">
-        <v>4.07</v>
-      </c>
-      <c r="O20" t="inlineStr">
+      <c r="S20" t="inlineStr">
         <is>
           <t>12/07/2023 22:12</t>
         </is>
       </c>
-      <c r="P20" t="n">
-        <v>3.27</v>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>14/07/2023 09:57</t>
-        </is>
-      </c>
-      <c r="R20" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>12/07/2023 22:12</t>
-        </is>
-      </c>
       <c r="T20" t="n">
-        <v>3.05</v>
+        <v>2.11</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>14/07/2023 09:58</t>
+          <t>14/07/2023 09:53</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-pss-sleman/nZin4VzL/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-psm-makassar/QPjj3kjR/</t>
         </is>
       </c>
     </row>
@@ -4253,22 +4253,22 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persis Solo</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Arema FC</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>2.32</v>
+        <v>1.65</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
@@ -4276,7 +4276,7 @@
         </is>
       </c>
       <c r="L42" t="n">
-        <v>2.79</v>
+        <v>1.61</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
@@ -4284,7 +4284,7 @@
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.26</v>
+        <v>3.8</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -4292,15 +4292,15 @@
         </is>
       </c>
       <c r="P42" t="n">
-        <v>3.5</v>
+        <v>4.15</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>30/07/2023 09:58</t>
+          <t>30/07/2023 09:55</t>
         </is>
       </c>
       <c r="R42" t="n">
-        <v>2.75</v>
+        <v>4.48</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
@@ -4308,16 +4308,16 @@
         </is>
       </c>
       <c r="T42" t="n">
-        <v>2.42</v>
+        <v>5.06</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>30/07/2023 09:55</t>
+          <t>30/07/2023 09:51</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-pss-sleman/pCUpNqs0/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persis-solo-arema-fc/tvOgLNBC/</t>
         </is>
       </c>
     </row>
@@ -4345,22 +4345,22 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Persis Solo</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Arema FC</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>1.65</v>
+        <v>2.32</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -4368,7 +4368,7 @@
         </is>
       </c>
       <c r="L43" t="n">
-        <v>1.61</v>
+        <v>2.79</v>
       </c>
       <c r="M43" t="inlineStr">
         <is>
@@ -4376,7 +4376,7 @@
         </is>
       </c>
       <c r="N43" t="n">
-        <v>3.8</v>
+        <v>3.26</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -4384,32 +4384,32 @@
         </is>
       </c>
       <c r="P43" t="n">
-        <v>4.15</v>
+        <v>3.5</v>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
+          <t>30/07/2023 09:58</t>
+        </is>
+      </c>
+      <c r="R43" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>28/07/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T43" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
           <t>30/07/2023 09:55</t>
         </is>
       </c>
-      <c r="R43" t="n">
-        <v>4.48</v>
-      </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>28/07/2023 22:12</t>
-        </is>
-      </c>
-      <c r="T43" t="n">
-        <v>5.06</v>
-      </c>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>30/07/2023 09:51</t>
-        </is>
-      </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persis-solo-arema-fc/tvOgLNBC/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-pss-sleman/pCUpNqs0/</t>
         </is>
       </c>
     </row>
@@ -7197,22 +7197,22 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>FC Bhayangkara</t>
         </is>
       </c>
       <c r="G74" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Borneo</t>
+        </is>
+      </c>
+      <c r="I74" t="n">
         <v>2</v>
       </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>PSS Sleman</t>
-        </is>
-      </c>
-      <c r="I74" t="n">
-        <v>3</v>
-      </c>
       <c r="J74" t="n">
-        <v>1.75</v>
+        <v>2.81</v>
       </c>
       <c r="K74" t="inlineStr">
         <is>
@@ -7220,15 +7220,15 @@
         </is>
       </c>
       <c r="L74" t="n">
-        <v>1.91</v>
+        <v>3.19</v>
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>18/08/2023 13:51</t>
+          <t>18/08/2023 13:59</t>
         </is>
       </c>
       <c r="N74" t="n">
-        <v>3.54</v>
+        <v>3.28</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -7236,15 +7236,15 @@
         </is>
       </c>
       <c r="P74" t="n">
-        <v>3.35</v>
+        <v>3.29</v>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>18/08/2023 13:51</t>
+          <t>18/08/2023 13:59</t>
         </is>
       </c>
       <c r="R74" t="n">
-        <v>4.19</v>
+        <v>2.32</v>
       </c>
       <c r="S74" t="inlineStr">
         <is>
@@ -7252,16 +7252,16 @@
         </is>
       </c>
       <c r="T74" t="n">
-        <v>4.25</v>
+        <v>2.28</v>
       </c>
       <c r="U74" t="inlineStr">
         <is>
-          <t>18/08/2023 13:51</t>
+          <t>18/08/2023 13:59</t>
         </is>
       </c>
       <c r="V74" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-pss-sleman/EmCFQw5k/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-borneo/dC1KPcKe/</t>
         </is>
       </c>
     </row>
@@ -7289,22 +7289,22 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>FC Bhayangkara</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J75" t="n">
-        <v>2.81</v>
+        <v>1.75</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
@@ -7312,15 +7312,15 @@
         </is>
       </c>
       <c r="L75" t="n">
-        <v>3.19</v>
+        <v>1.91</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>18/08/2023 13:59</t>
+          <t>18/08/2023 13:51</t>
         </is>
       </c>
       <c r="N75" t="n">
-        <v>3.28</v>
+        <v>3.54</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -7328,15 +7328,15 @@
         </is>
       </c>
       <c r="P75" t="n">
-        <v>3.29</v>
+        <v>3.35</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>18/08/2023 13:59</t>
+          <t>18/08/2023 13:51</t>
         </is>
       </c>
       <c r="R75" t="n">
-        <v>2.32</v>
+        <v>4.19</v>
       </c>
       <c r="S75" t="inlineStr">
         <is>
@@ -7344,16 +7344,16 @@
         </is>
       </c>
       <c r="T75" t="n">
-        <v>2.28</v>
+        <v>4.25</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>18/08/2023 13:59</t>
+          <t>18/08/2023 13:51</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-borneo/dC1KPcKe/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-pss-sleman/EmCFQw5k/</t>
         </is>
       </c>
     </row>
@@ -7933,22 +7933,22 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Persik Kediri</t>
+          <t>Madura United</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>FC Bhayangkara</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J82" t="n">
-        <v>2.11</v>
+        <v>1.76</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -7956,15 +7956,15 @@
         </is>
       </c>
       <c r="L82" t="n">
-        <v>1.86</v>
+        <v>1.59</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>25/08/2023 09:58</t>
+          <t>25/08/2023 09:55</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>3.28</v>
+        <v>3.57</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -7972,15 +7972,15 @@
         </is>
       </c>
       <c r="P82" t="n">
-        <v>3.69</v>
+        <v>4</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>25/08/2023 09:58</t>
+          <t>25/08/2023 09:55</t>
         </is>
       </c>
       <c r="R82" t="n">
-        <v>3.11</v>
+        <v>3.95</v>
       </c>
       <c r="S82" t="inlineStr">
         <is>
@@ -7988,16 +7988,16 @@
         </is>
       </c>
       <c r="T82" t="n">
-        <v>4.02</v>
+        <v>5.59</v>
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>25/08/2023 09:58</t>
+          <t>25/08/2023 09:55</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-psis-semarang/SjxkuwKr/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/madura-united-fc-bhayangkara/AFRgvcZl/</t>
         </is>
       </c>
     </row>
@@ -8025,22 +8025,22 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Madura United</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>FC Bhayangkara</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J83" t="n">
-        <v>1.76</v>
+        <v>2.11</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -8048,15 +8048,15 @@
         </is>
       </c>
       <c r="L83" t="n">
-        <v>1.59</v>
+        <v>1.86</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>25/08/2023 09:55</t>
+          <t>25/08/2023 09:58</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>3.57</v>
+        <v>3.28</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -8064,15 +8064,15 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>4</v>
+        <v>3.69</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>25/08/2023 09:55</t>
+          <t>25/08/2023 09:58</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>3.95</v>
+        <v>3.11</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
@@ -8080,16 +8080,16 @@
         </is>
       </c>
       <c r="T83" t="n">
-        <v>5.59</v>
+        <v>4.02</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>25/08/2023 09:55</t>
+          <t>25/08/2023 09:58</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/madura-united-fc-bhayangkara/AFRgvcZl/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-psis-semarang/SjxkuwKr/</t>
         </is>
       </c>
     </row>
@@ -8117,7 +8117,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -8125,14 +8125,14 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.85</v>
+        <v>3.11</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -8140,15 +8140,15 @@
         </is>
       </c>
       <c r="L84" t="n">
-        <v>1.64</v>
+        <v>2.6</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>25/08/2023 13:51</t>
+          <t>25/08/2023 13:59</t>
         </is>
       </c>
       <c r="N84" t="n">
-        <v>3.73</v>
+        <v>3.17</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -8156,15 +8156,15 @@
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.9</v>
+        <v>3.11</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>25/08/2023 13:51</t>
+          <t>25/08/2023 13:59</t>
         </is>
       </c>
       <c r="R84" t="n">
-        <v>3.51</v>
+        <v>2.15</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
@@ -8172,16 +8172,16 @@
         </is>
       </c>
       <c r="T84" t="n">
-        <v>5.27</v>
+        <v>2.84</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>25/08/2023 13:51</t>
+          <t>25/08/2023 13:59</t>
         </is>
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-persita/l6QcwHle/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/dewa-united-persija-jakarta/IuV1xy41/</t>
         </is>
       </c>
     </row>
@@ -8209,7 +8209,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="G85" t="n">
@@ -8217,14 +8217,14 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J85" t="n">
-        <v>3.11</v>
+        <v>1.85</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -8232,15 +8232,15 @@
         </is>
       </c>
       <c r="L85" t="n">
-        <v>2.6</v>
+        <v>1.64</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>25/08/2023 13:59</t>
+          <t>25/08/2023 13:51</t>
         </is>
       </c>
       <c r="N85" t="n">
-        <v>3.17</v>
+        <v>3.73</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -8248,15 +8248,15 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.11</v>
+        <v>3.9</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>25/08/2023 13:59</t>
+          <t>25/08/2023 13:51</t>
         </is>
       </c>
       <c r="R85" t="n">
-        <v>2.15</v>
+        <v>3.51</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
@@ -8264,16 +8264,16 @@
         </is>
       </c>
       <c r="T85" t="n">
-        <v>2.84</v>
+        <v>5.27</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>25/08/2023 13:59</t>
+          <t>25/08/2023 13:51</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/dewa-united-persija-jakarta/IuV1xy41/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-persita/l6QcwHle/</t>
         </is>
       </c>
     </row>
@@ -12073,7 +12073,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G127" t="n">
@@ -12081,11 +12081,11 @@
       </c>
       <c r="H127" t="inlineStr">
         <is>
-          <t>Persis Solo</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="I127" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J127" t="n">
         <v>2.54</v>
@@ -12096,15 +12096,15 @@
         </is>
       </c>
       <c r="L127" t="n">
-        <v>3.74</v>
+        <v>3.07</v>
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>06/10/2023 09:56</t>
+          <t>06/10/2023 09:52</t>
         </is>
       </c>
       <c r="N127" t="n">
-        <v>3.24</v>
+        <v>3.19</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -12112,15 +12112,15 @@
         </is>
       </c>
       <c r="P127" t="n">
-        <v>3.73</v>
+        <v>3.19</v>
       </c>
       <c r="Q127" t="inlineStr">
         <is>
-          <t>06/10/2023 09:58</t>
+          <t>06/10/2023 09:52</t>
         </is>
       </c>
       <c r="R127" t="n">
-        <v>2.52</v>
+        <v>2.54</v>
       </c>
       <c r="S127" t="inlineStr">
         <is>
@@ -12128,16 +12128,16 @@
         </is>
       </c>
       <c r="T127" t="n">
-        <v>1.92</v>
+        <v>2.39</v>
       </c>
       <c r="U127" t="inlineStr">
         <is>
-          <t>06/10/2023 09:56</t>
+          <t>06/10/2023 09:52</t>
         </is>
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-persis-solo/OE3fW2x4/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-psis-semarang/j15nYO7i/</t>
         </is>
       </c>
     </row>
@@ -12165,7 +12165,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G128" t="n">
@@ -12173,11 +12173,11 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>Persis Solo</t>
         </is>
       </c>
       <c r="I128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J128" t="n">
         <v>2.54</v>
@@ -12188,15 +12188,15 @@
         </is>
       </c>
       <c r="L128" t="n">
-        <v>3.07</v>
+        <v>3.74</v>
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>06/10/2023 09:52</t>
+          <t>06/10/2023 09:56</t>
         </is>
       </c>
       <c r="N128" t="n">
-        <v>3.19</v>
+        <v>3.24</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -12204,15 +12204,15 @@
         </is>
       </c>
       <c r="P128" t="n">
-        <v>3.19</v>
+        <v>3.73</v>
       </c>
       <c r="Q128" t="inlineStr">
         <is>
-          <t>06/10/2023 09:52</t>
+          <t>06/10/2023 09:58</t>
         </is>
       </c>
       <c r="R128" t="n">
-        <v>2.54</v>
+        <v>2.52</v>
       </c>
       <c r="S128" t="inlineStr">
         <is>
@@ -12220,16 +12220,16 @@
         </is>
       </c>
       <c r="T128" t="n">
-        <v>2.39</v>
+        <v>1.92</v>
       </c>
       <c r="U128" t="inlineStr">
         <is>
-          <t>06/10/2023 09:52</t>
+          <t>06/10/2023 09:56</t>
         </is>
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-psis-semarang/j15nYO7i/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-persis-solo/OE3fW2x4/</t>
         </is>
       </c>
     </row>
@@ -13177,22 +13177,22 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>FC Bhayangkara</t>
         </is>
       </c>
       <c r="G139" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Persik Kediri</t>
+          <t>Barito Putera</t>
         </is>
       </c>
       <c r="I139" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J139" t="n">
-        <v>2.52</v>
+        <v>2.53</v>
       </c>
       <c r="K139" t="inlineStr">
         <is>
@@ -13200,7 +13200,7 @@
         </is>
       </c>
       <c r="L139" t="n">
-        <v>2.28</v>
+        <v>2.9</v>
       </c>
       <c r="M139" t="inlineStr">
         <is>
@@ -13208,7 +13208,7 @@
         </is>
       </c>
       <c r="N139" t="n">
-        <v>3.09</v>
+        <v>3.21</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -13216,32 +13216,32 @@
         </is>
       </c>
       <c r="P139" t="n">
-        <v>3.29</v>
+        <v>3.22</v>
       </c>
       <c r="Q139" t="inlineStr">
         <is>
+          <t>21/10/2023 09:57</t>
+        </is>
+      </c>
+      <c r="R139" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>19/10/2023 21:12</t>
+        </is>
+      </c>
+      <c r="T139" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="U139" t="inlineStr">
+        <is>
           <t>21/10/2023 09:59</t>
         </is>
       </c>
-      <c r="R139" t="n">
-        <v>2.63</v>
-      </c>
-      <c r="S139" t="inlineStr">
-        <is>
-          <t>19/10/2023 21:12</t>
-        </is>
-      </c>
-      <c r="T139" t="n">
-        <v>3.17</v>
-      </c>
-      <c r="U139" t="inlineStr">
-        <is>
-          <t>21/10/2023 09:55</t>
-        </is>
-      </c>
       <c r="V139" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/pss-sleman-persik-kediri/nicrVDcR/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-ps-barito-putera/80bvWgrL/</t>
         </is>
       </c>
     </row>
@@ -13269,22 +13269,22 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>FC Bhayangkara</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="G140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Barito Putera</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="I140" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J140" t="n">
-        <v>2.53</v>
+        <v>2.52</v>
       </c>
       <c r="K140" t="inlineStr">
         <is>
@@ -13292,7 +13292,7 @@
         </is>
       </c>
       <c r="L140" t="n">
-        <v>2.9</v>
+        <v>2.28</v>
       </c>
       <c r="M140" t="inlineStr">
         <is>
@@ -13300,7 +13300,7 @@
         </is>
       </c>
       <c r="N140" t="n">
-        <v>3.21</v>
+        <v>3.09</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -13308,15 +13308,15 @@
         </is>
       </c>
       <c r="P140" t="n">
-        <v>3.22</v>
+        <v>3.29</v>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
-          <t>21/10/2023 09:57</t>
+          <t>21/10/2023 09:59</t>
         </is>
       </c>
       <c r="R140" t="n">
-        <v>2.53</v>
+        <v>2.63</v>
       </c>
       <c r="S140" t="inlineStr">
         <is>
@@ -13324,16 +13324,16 @@
         </is>
       </c>
       <c r="T140" t="n">
-        <v>2.49</v>
+        <v>3.17</v>
       </c>
       <c r="U140" t="inlineStr">
         <is>
-          <t>21/10/2023 09:59</t>
+          <t>21/10/2023 09:55</t>
         </is>
       </c>
       <c r="V140" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-ps-barito-putera/80bvWgrL/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/pss-sleman-persik-kediri/nicrVDcR/</t>
         </is>
       </c>
     </row>
@@ -15726,6 +15726,190 @@
       <c r="V166" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/indonesia/liga-1/psis-semarang-persita/WtWvnllP/</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>indonesia</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>liga-1</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E167" s="2" t="n">
+        <v>45239.54166666666</v>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Persija Jakarta</t>
+        </is>
+      </c>
+      <c r="G167" t="n">
+        <v>4</v>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>Persikabo 1973</t>
+        </is>
+      </c>
+      <c r="I167" t="n">
+        <v>0</v>
+      </c>
+      <c r="J167" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L167" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="M167" t="inlineStr">
+        <is>
+          <t>09/11/2023 12:57</t>
+        </is>
+      </c>
+      <c r="N167" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="O167" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P167" t="n">
+        <v>4.39</v>
+      </c>
+      <c r="Q167" t="inlineStr">
+        <is>
+          <t>09/11/2023 12:59</t>
+        </is>
+      </c>
+      <c r="R167" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="S167" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T167" t="n">
+        <v>6.39</v>
+      </c>
+      <c r="U167" t="inlineStr">
+        <is>
+          <t>09/11/2023 12:59</t>
+        </is>
+      </c>
+      <c r="V167" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persija-jakarta-persikabo-1973/YkI6s8dt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>indonesia</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>liga-1</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E168" s="2" t="n">
+        <v>45239.54166666666</v>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>RANS Nusantara</t>
+        </is>
+      </c>
+      <c r="G168" t="n">
+        <v>1</v>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>FC Bhayangkara</t>
+        </is>
+      </c>
+      <c r="I168" t="n">
+        <v>1</v>
+      </c>
+      <c r="J168" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="L168" t="n">
+        <v>1.94</v>
+      </c>
+      <c r="M168" t="inlineStr">
+        <is>
+          <t>09/11/2023 12:58</t>
+        </is>
+      </c>
+      <c r="N168" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="O168" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="P168" t="n">
+        <v>3.59</v>
+      </c>
+      <c r="Q168" t="inlineStr">
+        <is>
+          <t>09/11/2023 12:54</t>
+        </is>
+      </c>
+      <c r="R168" t="n">
+        <v>3.32</v>
+      </c>
+      <c r="S168" t="inlineStr">
+        <is>
+          <t>08/11/2023 01:12</t>
+        </is>
+      </c>
+      <c r="T168" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="U168" t="inlineStr">
+        <is>
+          <t>09/11/2023 12:58</t>
+        </is>
+      </c>
+      <c r="V168" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-fc-bhayangkara/tGLEunRh/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 02-12-2023 08:45
</commit_message>
<xml_diff>
--- a/2023/indonesia_liga-1_2023-2024.xlsx
+++ b/2023/indonesia_liga-1_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V179"/>
+  <dimension ref="A1:V181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1953,22 +1953,22 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>FC Bhayangkara</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>1.32</v>
+        <v>3.34</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
@@ -1976,15 +1976,15 @@
         </is>
       </c>
       <c r="L17" t="n">
-        <v>1.75</v>
+        <v>4.55</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>09/07/2023 13:54</t>
+          <t>09/07/2023 13:59</t>
         </is>
       </c>
       <c r="N17" t="n">
-        <v>5.37</v>
+        <v>3.3</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1992,15 +1992,15 @@
         </is>
       </c>
       <c r="P17" t="n">
-        <v>3.97</v>
+        <v>3.38</v>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>09/07/2023 13:54</t>
+          <t>09/07/2023 13:59</t>
         </is>
       </c>
       <c r="R17" t="n">
-        <v>6.1</v>
+        <v>1.99</v>
       </c>
       <c r="S17" t="inlineStr">
         <is>
@@ -2008,16 +2008,16 @@
         </is>
       </c>
       <c r="T17" t="n">
-        <v>4.29</v>
+        <v>1.85</v>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>09/07/2023 13:54</t>
+          <t>09/07/2023 13:59</t>
         </is>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-rans-nusantara/6Nzk5BLE/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-persija-jakarta/SWyo6i68/</t>
         </is>
       </c>
     </row>
@@ -2045,22 +2045,22 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>FC Bhayangkara</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18" t="n">
-        <v>3.34</v>
+        <v>1.32</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -2068,15 +2068,15 @@
         </is>
       </c>
       <c r="L18" t="n">
-        <v>4.55</v>
+        <v>1.75</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>09/07/2023 13:59</t>
+          <t>09/07/2023 13:54</t>
         </is>
       </c>
       <c r="N18" t="n">
-        <v>3.3</v>
+        <v>5.37</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -2084,15 +2084,15 @@
         </is>
       </c>
       <c r="P18" t="n">
-        <v>3.38</v>
+        <v>3.97</v>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>09/07/2023 13:59</t>
+          <t>09/07/2023 13:54</t>
         </is>
       </c>
       <c r="R18" t="n">
-        <v>1.99</v>
+        <v>6.1</v>
       </c>
       <c r="S18" t="inlineStr">
         <is>
@@ -2100,16 +2100,16 @@
         </is>
       </c>
       <c r="T18" t="n">
-        <v>1.85</v>
+        <v>4.29</v>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>09/07/2023 13:59</t>
+          <t>09/07/2023 13:54</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-persija-jakarta/SWyo6i68/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-rans-nusantara/6Nzk5BLE/</t>
         </is>
       </c>
     </row>
@@ -2137,22 +2137,22 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Barito Putera</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>PSM Makassar</t>
         </is>
       </c>
       <c r="I19" t="n">
         <v>1</v>
       </c>
       <c r="J19" t="n">
-        <v>1.56</v>
+        <v>3.73</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
@@ -2160,48 +2160,48 @@
         </is>
       </c>
       <c r="L19" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>14/07/2023 09:53</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>12/07/2023 22:12</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>14/07/2023 09:53</t>
+        </is>
+      </c>
+      <c r="R19" t="n">
         <v>1.86</v>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>14/07/2023 09:58</t>
-        </is>
-      </c>
-      <c r="N19" t="n">
-        <v>4.07</v>
-      </c>
-      <c r="O19" t="inlineStr">
+      <c r="S19" t="inlineStr">
         <is>
           <t>12/07/2023 22:12</t>
         </is>
       </c>
-      <c r="P19" t="n">
-        <v>3.27</v>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>14/07/2023 09:57</t>
-        </is>
-      </c>
-      <c r="R19" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>12/07/2023 22:12</t>
-        </is>
-      </c>
       <c r="T19" t="n">
-        <v>3.05</v>
+        <v>2.11</v>
       </c>
       <c r="U19" t="inlineStr">
         <is>
-          <t>14/07/2023 09:58</t>
+          <t>14/07/2023 09:53</t>
         </is>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-pss-sleman/nZin4VzL/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-psm-makassar/QPjj3kjR/</t>
         </is>
       </c>
     </row>
@@ -2229,22 +2229,22 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>Barito Putera</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>PSM Makassar</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I20" t="n">
         <v>1</v>
       </c>
       <c r="J20" t="n">
-        <v>3.73</v>
+        <v>1.56</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
@@ -2252,15 +2252,15 @@
         </is>
       </c>
       <c r="L20" t="n">
-        <v>3.53</v>
+        <v>1.86</v>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>14/07/2023 09:53</t>
+          <t>14/07/2023 09:58</t>
         </is>
       </c>
       <c r="N20" t="n">
-        <v>3.49</v>
+        <v>4.07</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -2268,15 +2268,15 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>3.33</v>
+        <v>3.27</v>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>14/07/2023 09:53</t>
+          <t>14/07/2023 09:57</t>
         </is>
       </c>
       <c r="R20" t="n">
-        <v>1.86</v>
+        <v>4.9</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
@@ -2284,16 +2284,16 @@
         </is>
       </c>
       <c r="T20" t="n">
-        <v>2.11</v>
+        <v>3.05</v>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>14/07/2023 09:53</t>
+          <t>14/07/2023 09:58</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persikabo-1973-psm-makassar/QPjj3kjR/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-pss-sleman/nZin4VzL/</t>
         </is>
       </c>
     </row>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -2973,14 +2973,14 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>Barito Putera</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28" t="n">
-        <v>2.97</v>
+        <v>1.6</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
@@ -2988,15 +2988,15 @@
         </is>
       </c>
       <c r="L28" t="n">
-        <v>2.09</v>
+        <v>1.58</v>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>21/07/2023 09:54</t>
+          <t>21/07/2023 09:58</t>
         </is>
       </c>
       <c r="N28" t="n">
-        <v>3.28</v>
+        <v>4</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -3004,15 +3004,15 @@
         </is>
       </c>
       <c r="P28" t="n">
-        <v>3.44</v>
+        <v>4.19</v>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>21/07/2023 09:54</t>
+          <t>21/07/2023 09:59</t>
         </is>
       </c>
       <c r="R28" t="n">
-        <v>2.22</v>
+        <v>4.64</v>
       </c>
       <c r="S28" t="inlineStr">
         <is>
@@ -3020,16 +3020,16 @@
         </is>
       </c>
       <c r="T28" t="n">
-        <v>3.47</v>
+        <v>5.33</v>
       </c>
       <c r="U28" t="inlineStr">
         <is>
-          <t>21/07/2023 09:54</t>
+          <t>21/07/2023 09:59</t>
         </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/pss-sleman-psis-semarang/Qme89QC0/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-ps-barito-putera/vTGPHl5K/</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -3065,14 +3065,14 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Barito Putera</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J29" t="n">
-        <v>1.6</v>
+        <v>2.97</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -3080,15 +3080,15 @@
         </is>
       </c>
       <c r="L29" t="n">
-        <v>1.58</v>
+        <v>2.09</v>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>21/07/2023 09:58</t>
+          <t>21/07/2023 09:54</t>
         </is>
       </c>
       <c r="N29" t="n">
-        <v>4</v>
+        <v>3.28</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -3096,15 +3096,15 @@
         </is>
       </c>
       <c r="P29" t="n">
-        <v>4.19</v>
+        <v>3.44</v>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>21/07/2023 09:59</t>
+          <t>21/07/2023 09:54</t>
         </is>
       </c>
       <c r="R29" t="n">
-        <v>4.64</v>
+        <v>2.22</v>
       </c>
       <c r="S29" t="inlineStr">
         <is>
@@ -3112,16 +3112,16 @@
         </is>
       </c>
       <c r="T29" t="n">
-        <v>5.33</v>
+        <v>3.47</v>
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>21/07/2023 09:59</t>
+          <t>21/07/2023 09:54</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-ps-barito-putera/vTGPHl5K/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/pss-sleman-psis-semarang/Qme89QC0/</t>
         </is>
       </c>
     </row>
@@ -3149,19 +3149,19 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Arema FC</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Bali United</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
         <v>2.7</v>
@@ -3172,15 +3172,15 @@
         </is>
       </c>
       <c r="L30" t="n">
-        <v>4.79</v>
+        <v>2.53</v>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>21/07/2023 13:59</t>
+          <t>21/07/2023 13:57</t>
         </is>
       </c>
       <c r="N30" t="n">
-        <v>3.28</v>
+        <v>3.13</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -3188,15 +3188,15 @@
         </is>
       </c>
       <c r="P30" t="n">
-        <v>3.86</v>
+        <v>3.69</v>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>21/07/2023 13:58</t>
+          <t>21/07/2023 13:57</t>
         </is>
       </c>
       <c r="R30" t="n">
-        <v>2.35</v>
+        <v>2.44</v>
       </c>
       <c r="S30" t="inlineStr">
         <is>
@@ -3204,16 +3204,16 @@
         </is>
       </c>
       <c r="T30" t="n">
-        <v>1.69</v>
+        <v>2.55</v>
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>21/07/2023 13:54</t>
+          <t>21/07/2023 13:57</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/arema-fc-bali-united/za2eCSSs/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/dewa-united-persik-kediri/YkGTG8KQ/</t>
         </is>
       </c>
     </row>
@@ -3241,19 +3241,19 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>Arema FC</t>
         </is>
       </c>
       <c r="G31" t="n">
+        <v>1</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Bali United</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
         <v>3</v>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Persik Kediri</t>
-        </is>
-      </c>
-      <c r="I31" t="n">
-        <v>0</v>
       </c>
       <c r="J31" t="n">
         <v>2.7</v>
@@ -3264,15 +3264,15 @@
         </is>
       </c>
       <c r="L31" t="n">
-        <v>2.53</v>
+        <v>4.79</v>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>21/07/2023 13:57</t>
+          <t>21/07/2023 13:59</t>
         </is>
       </c>
       <c r="N31" t="n">
-        <v>3.13</v>
+        <v>3.28</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -3280,15 +3280,15 @@
         </is>
       </c>
       <c r="P31" t="n">
-        <v>3.69</v>
+        <v>3.86</v>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>21/07/2023 13:57</t>
+          <t>21/07/2023 13:58</t>
         </is>
       </c>
       <c r="R31" t="n">
-        <v>2.44</v>
+        <v>2.35</v>
       </c>
       <c r="S31" t="inlineStr">
         <is>
@@ -3296,16 +3296,16 @@
         </is>
       </c>
       <c r="T31" t="n">
-        <v>2.55</v>
+        <v>1.69</v>
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>21/07/2023 13:57</t>
+          <t>21/07/2023 13:54</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/dewa-united-persik-kediri/YkGTG8KQ/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/arema-fc-bali-united/za2eCSSs/</t>
         </is>
       </c>
     </row>
@@ -4253,22 +4253,22 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persis Solo</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Arema FC</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="n">
-        <v>2.32</v>
+        <v>1.65</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
@@ -4276,7 +4276,7 @@
         </is>
       </c>
       <c r="L42" t="n">
-        <v>2.79</v>
+        <v>1.61</v>
       </c>
       <c r="M42" t="inlineStr">
         <is>
@@ -4284,7 +4284,7 @@
         </is>
       </c>
       <c r="N42" t="n">
-        <v>3.26</v>
+        <v>3.8</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -4292,15 +4292,15 @@
         </is>
       </c>
       <c r="P42" t="n">
-        <v>3.5</v>
+        <v>4.15</v>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>30/07/2023 09:58</t>
+          <t>30/07/2023 09:55</t>
         </is>
       </c>
       <c r="R42" t="n">
-        <v>2.75</v>
+        <v>4.48</v>
       </c>
       <c r="S42" t="inlineStr">
         <is>
@@ -4308,16 +4308,16 @@
         </is>
       </c>
       <c r="T42" t="n">
-        <v>2.42</v>
+        <v>5.06</v>
       </c>
       <c r="U42" t="inlineStr">
         <is>
-          <t>30/07/2023 09:55</t>
+          <t>30/07/2023 09:51</t>
         </is>
       </c>
       <c r="V42" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-pss-sleman/pCUpNqs0/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persis-solo-arema-fc/tvOgLNBC/</t>
         </is>
       </c>
     </row>
@@ -4345,22 +4345,22 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Persis Solo</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Arema FC</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="n">
-        <v>1.65</v>
+        <v>2.32</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
@@ -4368,7 +4368,7 @@
         </is>
       </c>
       <c r="L43" t="n">
-        <v>1.61</v>
+        <v>2.79</v>
       </c>
       <c r="M43" t="inlineStr">
         <is>
@@ -4376,7 +4376,7 @@
         </is>
       </c>
       <c r="N43" t="n">
-        <v>3.8</v>
+        <v>3.26</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -4384,32 +4384,32 @@
         </is>
       </c>
       <c r="P43" t="n">
-        <v>4.15</v>
+        <v>3.5</v>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
+          <t>30/07/2023 09:58</t>
+        </is>
+      </c>
+      <c r="R43" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>28/07/2023 22:12</t>
+        </is>
+      </c>
+      <c r="T43" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
           <t>30/07/2023 09:55</t>
         </is>
       </c>
-      <c r="R43" t="n">
-        <v>4.48</v>
-      </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>28/07/2023 22:12</t>
-        </is>
-      </c>
-      <c r="T43" t="n">
-        <v>5.06</v>
-      </c>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>30/07/2023 09:51</t>
-        </is>
-      </c>
       <c r="V43" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persis-solo-arema-fc/tvOgLNBC/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-pss-sleman/pCUpNqs0/</t>
         </is>
       </c>
     </row>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>Barito Putera</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -4445,14 +4445,14 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Persebaya</t>
+          <t>Madura United</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J44" t="n">
-        <v>1.62</v>
+        <v>2.12</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
@@ -4460,15 +4460,15 @@
         </is>
       </c>
       <c r="L44" t="n">
-        <v>1.67</v>
+        <v>2.34</v>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>30/07/2023 13:52</t>
+          <t>30/07/2023 13:51</t>
         </is>
       </c>
       <c r="N44" t="n">
-        <v>3.93</v>
+        <v>3.31</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -4476,15 +4476,15 @@
         </is>
       </c>
       <c r="P44" t="n">
-        <v>3.9</v>
+        <v>3.44</v>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>30/07/2023 13:52</t>
+          <t>30/07/2023 13:51</t>
         </is>
       </c>
       <c r="R44" t="n">
-        <v>4.54</v>
+        <v>3.13</v>
       </c>
       <c r="S44" t="inlineStr">
         <is>
@@ -4492,16 +4492,16 @@
         </is>
       </c>
       <c r="T44" t="n">
-        <v>4.97</v>
+        <v>2.94</v>
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>30/07/2023 13:52</t>
+          <t>30/07/2023 13:51</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persija-jakarta-persebaya/2mPkM3d6/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-madura-united/z1NcKsRI/</t>
         </is>
       </c>
     </row>
@@ -4529,7 +4529,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Barito Putera</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -4537,14 +4537,14 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Madura United</t>
+          <t>Persebaya</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>2.12</v>
+        <v>1.62</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
@@ -4552,15 +4552,15 @@
         </is>
       </c>
       <c r="L45" t="n">
-        <v>2.34</v>
+        <v>1.67</v>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>30/07/2023 13:51</t>
+          <t>30/07/2023 13:52</t>
         </is>
       </c>
       <c r="N45" t="n">
-        <v>3.31</v>
+        <v>3.93</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -4568,15 +4568,15 @@
         </is>
       </c>
       <c r="P45" t="n">
-        <v>3.44</v>
+        <v>3.9</v>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>30/07/2023 13:51</t>
+          <t>30/07/2023 13:52</t>
         </is>
       </c>
       <c r="R45" t="n">
-        <v>3.13</v>
+        <v>4.54</v>
       </c>
       <c r="S45" t="inlineStr">
         <is>
@@ -4584,16 +4584,16 @@
         </is>
       </c>
       <c r="T45" t="n">
-        <v>2.94</v>
+        <v>4.97</v>
       </c>
       <c r="U45" t="inlineStr">
         <is>
-          <t>30/07/2023 13:51</t>
+          <t>30/07/2023 13:52</t>
         </is>
       </c>
       <c r="V45" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-madura-united/z1NcKsRI/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persija-jakarta-persebaya/2mPkM3d6/</t>
         </is>
       </c>
     </row>
@@ -7933,22 +7933,22 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Madura United</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>FC Bhayangkara</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J82" t="n">
-        <v>1.76</v>
+        <v>2.11</v>
       </c>
       <c r="K82" t="inlineStr">
         <is>
@@ -7956,15 +7956,15 @@
         </is>
       </c>
       <c r="L82" t="n">
-        <v>1.59</v>
+        <v>1.86</v>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>25/08/2023 09:55</t>
+          <t>25/08/2023 09:58</t>
         </is>
       </c>
       <c r="N82" t="n">
-        <v>3.57</v>
+        <v>3.28</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -7972,15 +7972,15 @@
         </is>
       </c>
       <c r="P82" t="n">
-        <v>4</v>
+        <v>3.69</v>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>25/08/2023 09:55</t>
+          <t>25/08/2023 09:58</t>
         </is>
       </c>
       <c r="R82" t="n">
-        <v>3.95</v>
+        <v>3.11</v>
       </c>
       <c r="S82" t="inlineStr">
         <is>
@@ -7988,16 +7988,16 @@
         </is>
       </c>
       <c r="T82" t="n">
-        <v>5.59</v>
+        <v>4.02</v>
       </c>
       <c r="U82" t="inlineStr">
         <is>
-          <t>25/08/2023 09:55</t>
+          <t>25/08/2023 09:58</t>
         </is>
       </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/madura-united-fc-bhayangkara/AFRgvcZl/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-psis-semarang/SjxkuwKr/</t>
         </is>
       </c>
     </row>
@@ -8025,22 +8025,22 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Persik Kediri</t>
+          <t>Madura United</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>FC Bhayangkara</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J83" t="n">
-        <v>2.11</v>
+        <v>1.76</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -8048,15 +8048,15 @@
         </is>
       </c>
       <c r="L83" t="n">
-        <v>1.86</v>
+        <v>1.59</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>25/08/2023 09:58</t>
+          <t>25/08/2023 09:55</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>3.28</v>
+        <v>3.57</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -8064,15 +8064,15 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>3.69</v>
+        <v>4</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>25/08/2023 09:58</t>
+          <t>25/08/2023 09:55</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>3.11</v>
+        <v>3.95</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
@@ -8080,16 +8080,16 @@
         </is>
       </c>
       <c r="T83" t="n">
-        <v>4.02</v>
+        <v>5.59</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>25/08/2023 09:58</t>
+          <t>25/08/2023 09:55</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-psis-semarang/SjxkuwKr/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/madura-united-fc-bhayangkara/AFRgvcZl/</t>
         </is>
       </c>
     </row>
@@ -8117,7 +8117,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="G84" t="n">
@@ -8125,14 +8125,14 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J84" t="n">
-        <v>1.85</v>
+        <v>3.11</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -8140,15 +8140,15 @@
         </is>
       </c>
       <c r="L84" t="n">
-        <v>1.64</v>
+        <v>2.6</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>25/08/2023 13:51</t>
+          <t>25/08/2023 13:59</t>
         </is>
       </c>
       <c r="N84" t="n">
-        <v>3.73</v>
+        <v>3.17</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -8156,15 +8156,15 @@
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.9</v>
+        <v>3.11</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>25/08/2023 13:51</t>
+          <t>25/08/2023 13:59</t>
         </is>
       </c>
       <c r="R84" t="n">
-        <v>3.51</v>
+        <v>2.15</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
@@ -8172,16 +8172,16 @@
         </is>
       </c>
       <c r="T84" t="n">
-        <v>5.27</v>
+        <v>2.84</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>25/08/2023 13:51</t>
+          <t>25/08/2023 13:59</t>
         </is>
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-persita/l6QcwHle/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/dewa-united-persija-jakarta/IuV1xy41/</t>
         </is>
       </c>
     </row>
@@ -8209,7 +8209,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="G85" t="n">
@@ -8217,14 +8217,14 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J85" t="n">
-        <v>3.11</v>
+        <v>1.85</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -8232,15 +8232,15 @@
         </is>
       </c>
       <c r="L85" t="n">
-        <v>2.6</v>
+        <v>1.64</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>25/08/2023 13:59</t>
+          <t>25/08/2023 13:51</t>
         </is>
       </c>
       <c r="N85" t="n">
-        <v>3.17</v>
+        <v>3.73</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -8248,15 +8248,15 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.11</v>
+        <v>3.9</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>25/08/2023 13:59</t>
+          <t>25/08/2023 13:51</t>
         </is>
       </c>
       <c r="R85" t="n">
-        <v>2.15</v>
+        <v>3.51</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
@@ -8264,16 +8264,16 @@
         </is>
       </c>
       <c r="T85" t="n">
-        <v>2.84</v>
+        <v>5.27</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>25/08/2023 13:59</t>
+          <t>25/08/2023 13:51</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/dewa-united-persija-jakarta/IuV1xy41/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-persita/l6QcwHle/</t>
         </is>
       </c>
     </row>
@@ -8945,7 +8945,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="G93" t="n">
@@ -8953,14 +8953,14 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Persib Bandung</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="I93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J93" t="n">
-        <v>1.96</v>
+        <v>2.42</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
@@ -8968,15 +8968,15 @@
         </is>
       </c>
       <c r="L93" t="n">
-        <v>1.96</v>
+        <v>2.2</v>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>02/09/2023 09:57</t>
+          <t>02/09/2023 09:51</t>
         </is>
       </c>
       <c r="N93" t="n">
-        <v>3.33</v>
+        <v>3.25</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
@@ -8984,15 +8984,15 @@
         </is>
       </c>
       <c r="P93" t="n">
-        <v>3.19</v>
+        <v>3.16</v>
       </c>
       <c r="Q93" t="inlineStr">
         <is>
-          <t>02/09/2023 09:57</t>
+          <t>02/09/2023 09:51</t>
         </is>
       </c>
       <c r="R93" t="n">
-        <v>3.44</v>
+        <v>2.7</v>
       </c>
       <c r="S93" t="inlineStr">
         <is>
@@ -9000,16 +9000,16 @@
         </is>
       </c>
       <c r="T93" t="n">
-        <v>4.27</v>
+        <v>3.5</v>
       </c>
       <c r="U93" t="inlineStr">
         <is>
-          <t>02/09/2023 09:57</t>
+          <t>02/09/2023 09:51</t>
         </is>
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persija-jakarta-persib-bandung/vTdwxS9I/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-persik-kediri/d47Yx8fC/</t>
         </is>
       </c>
     </row>
@@ -9037,7 +9037,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="G94" t="n">
@@ -9045,14 +9045,14 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>Persik Kediri</t>
+          <t>Persib Bandung</t>
         </is>
       </c>
       <c r="I94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J94" t="n">
-        <v>2.42</v>
+        <v>1.96</v>
       </c>
       <c r="K94" t="inlineStr">
         <is>
@@ -9060,15 +9060,15 @@
         </is>
       </c>
       <c r="L94" t="n">
-        <v>2.2</v>
+        <v>1.96</v>
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>02/09/2023 09:51</t>
+          <t>02/09/2023 09:57</t>
         </is>
       </c>
       <c r="N94" t="n">
-        <v>3.25</v>
+        <v>3.33</v>
       </c>
       <c r="O94" t="inlineStr">
         <is>
@@ -9076,15 +9076,15 @@
         </is>
       </c>
       <c r="P94" t="n">
-        <v>3.16</v>
+        <v>3.19</v>
       </c>
       <c r="Q94" t="inlineStr">
         <is>
-          <t>02/09/2023 09:51</t>
+          <t>02/09/2023 09:57</t>
         </is>
       </c>
       <c r="R94" t="n">
-        <v>2.7</v>
+        <v>3.44</v>
       </c>
       <c r="S94" t="inlineStr">
         <is>
@@ -9092,16 +9092,16 @@
         </is>
       </c>
       <c r="T94" t="n">
-        <v>3.5</v>
+        <v>4.27</v>
       </c>
       <c r="U94" t="inlineStr">
         <is>
-          <t>02/09/2023 09:51</t>
+          <t>02/09/2023 09:57</t>
         </is>
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-persik-kediri/d47Yx8fC/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persija-jakarta-persib-bandung/vTdwxS9I/</t>
         </is>
       </c>
     </row>
@@ -9865,71 +9865,71 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Persib Bandung</t>
+          <t>Arema FC</t>
         </is>
       </c>
       <c r="G103" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="I103" t="n">
         <v>0</v>
       </c>
       <c r="J103" t="n">
-        <v>1.37</v>
+        <v>2.63</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>14/09/2023 22:12</t>
+          <t>14/09/2023 22:13</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>1.49</v>
+        <v>2.66</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>16/09/2023 09:53</t>
+          <t>16/09/2023 09:54</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>4.64</v>
+        <v>3.06</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>14/09/2023 22:12</t>
+          <t>14/09/2023 22:13</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>4.42</v>
+        <v>3.13</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>16/09/2023 09:53</t>
+          <t>16/09/2023 09:51</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>6.41</v>
+        <v>2.54</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>14/09/2023 22:12</t>
+          <t>14/09/2023 22:13</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>6.27</v>
+        <v>2.76</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>16/09/2023 09:53</t>
+          <t>16/09/2023 09:54</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persib-bandung-persikabo-1973/WMLGkovI/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/arema-fc-persita/hWMCjROB/</t>
         </is>
       </c>
     </row>
@@ -9957,71 +9957,71 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Arema FC</t>
+          <t>Persib Bandung</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="I104" t="n">
         <v>0</v>
       </c>
       <c r="J104" t="n">
-        <v>2.63</v>
+        <v>1.37</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>14/09/2023 22:13</t>
+          <t>14/09/2023 22:12</t>
         </is>
       </c>
       <c r="L104" t="n">
-        <v>2.66</v>
+        <v>1.49</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>16/09/2023 09:54</t>
+          <t>16/09/2023 09:53</t>
         </is>
       </c>
       <c r="N104" t="n">
-        <v>3.06</v>
+        <v>4.64</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
-          <t>14/09/2023 22:13</t>
+          <t>14/09/2023 22:12</t>
         </is>
       </c>
       <c r="P104" t="n">
-        <v>3.13</v>
+        <v>4.42</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>16/09/2023 09:51</t>
+          <t>16/09/2023 09:53</t>
         </is>
       </c>
       <c r="R104" t="n">
-        <v>2.54</v>
+        <v>6.41</v>
       </c>
       <c r="S104" t="inlineStr">
         <is>
-          <t>14/09/2023 22:13</t>
+          <t>14/09/2023 22:12</t>
         </is>
       </c>
       <c r="T104" t="n">
-        <v>2.76</v>
+        <v>6.27</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
-          <t>16/09/2023 09:54</t>
+          <t>16/09/2023 09:53</t>
         </is>
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/arema-fc-persita/hWMCjROB/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persib-bandung-persikabo-1973/WMLGkovI/</t>
         </is>
       </c>
     </row>
@@ -10233,7 +10233,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="G107" t="n">
@@ -10241,14 +10241,14 @@
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Persija Jakarta</t>
         </is>
       </c>
       <c r="I107" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J107" t="n">
-        <v>1.56</v>
+        <v>2.82</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -10256,15 +10256,15 @@
         </is>
       </c>
       <c r="L107" t="n">
-        <v>1.5</v>
+        <v>3.07</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>17/09/2023 13:53</t>
+          <t>17/09/2023 13:52</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>4.05</v>
+        <v>3.09</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -10272,15 +10272,15 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>4.47</v>
+        <v>2.94</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>17/09/2023 13:53</t>
+          <t>17/09/2023 13:52</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>4.92</v>
+        <v>2.37</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
@@ -10288,16 +10288,16 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>6.08</v>
+        <v>2.55</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>17/09/2023 13:53</t>
+          <t>17/09/2023 13:52</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-pss-sleman/4AjV88vt/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-persija-jakarta/r1kZ7Sgn/</t>
         </is>
       </c>
     </row>
@@ -10325,7 +10325,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Persik Kediri</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="G108" t="n">
@@ -10333,14 +10333,14 @@
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>Persija Jakarta</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I108" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J108" t="n">
-        <v>2.82</v>
+        <v>1.56</v>
       </c>
       <c r="K108" t="inlineStr">
         <is>
@@ -10348,15 +10348,15 @@
         </is>
       </c>
       <c r="L108" t="n">
-        <v>3.07</v>
+        <v>1.5</v>
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>17/09/2023 13:52</t>
+          <t>17/09/2023 13:53</t>
         </is>
       </c>
       <c r="N108" t="n">
-        <v>3.09</v>
+        <v>4.05</v>
       </c>
       <c r="O108" t="inlineStr">
         <is>
@@ -10364,15 +10364,15 @@
         </is>
       </c>
       <c r="P108" t="n">
-        <v>2.94</v>
+        <v>4.47</v>
       </c>
       <c r="Q108" t="inlineStr">
         <is>
-          <t>17/09/2023 13:52</t>
+          <t>17/09/2023 13:53</t>
         </is>
       </c>
       <c r="R108" t="n">
-        <v>2.37</v>
+        <v>4.92</v>
       </c>
       <c r="S108" t="inlineStr">
         <is>
@@ -10380,16 +10380,16 @@
         </is>
       </c>
       <c r="T108" t="n">
-        <v>2.55</v>
+        <v>6.08</v>
       </c>
       <c r="U108" t="inlineStr">
         <is>
-          <t>17/09/2023 13:52</t>
+          <t>17/09/2023 13:53</t>
         </is>
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-persija-jakarta/r1kZ7Sgn/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-pss-sleman/4AjV88vt/</t>
         </is>
       </c>
     </row>
@@ -12717,22 +12717,22 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>FC Bhayangkara</t>
         </is>
       </c>
       <c r="G134" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>Persik Kediri</t>
+          <t>Bali United</t>
         </is>
       </c>
       <c r="I134" t="n">
         <v>2</v>
       </c>
       <c r="J134" t="n">
-        <v>2.18</v>
+        <v>2.71</v>
       </c>
       <c r="K134" t="inlineStr">
         <is>
@@ -12740,15 +12740,15 @@
         </is>
       </c>
       <c r="L134" t="n">
-        <v>2.07</v>
+        <v>3.01</v>
       </c>
       <c r="M134" t="inlineStr">
         <is>
-          <t>08/10/2023 13:53</t>
+          <t>08/10/2023 13:51</t>
         </is>
       </c>
       <c r="N134" t="n">
-        <v>3.22</v>
+        <v>3.33</v>
       </c>
       <c r="O134" t="inlineStr">
         <is>
@@ -12756,15 +12756,15 @@
         </is>
       </c>
       <c r="P134" t="n">
-        <v>3.22</v>
+        <v>3.52</v>
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>08/10/2023 13:53</t>
+          <t>08/10/2023 12:26</t>
         </is>
       </c>
       <c r="R134" t="n">
-        <v>3.02</v>
+        <v>2.31</v>
       </c>
       <c r="S134" t="inlineStr">
         <is>
@@ -12772,16 +12772,16 @@
         </is>
       </c>
       <c r="T134" t="n">
-        <v>3.8</v>
+        <v>2.27</v>
       </c>
       <c r="U134" t="inlineStr">
         <is>
-          <t>08/10/2023 13:53</t>
+          <t>08/10/2023 13:51</t>
         </is>
       </c>
       <c r="V134" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-persik-kediri/QuPzCYjk/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-bali-united/neDqACL1/</t>
         </is>
       </c>
     </row>
@@ -12809,22 +12809,22 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>FC Bhayangkara</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="G135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>Bali United</t>
+          <t>Persik Kediri</t>
         </is>
       </c>
       <c r="I135" t="n">
         <v>2</v>
       </c>
       <c r="J135" t="n">
-        <v>2.71</v>
+        <v>2.18</v>
       </c>
       <c r="K135" t="inlineStr">
         <is>
@@ -12832,15 +12832,15 @@
         </is>
       </c>
       <c r="L135" t="n">
-        <v>3.01</v>
+        <v>2.07</v>
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>08/10/2023 13:51</t>
+          <t>08/10/2023 13:53</t>
         </is>
       </c>
       <c r="N135" t="n">
-        <v>3.33</v>
+        <v>3.22</v>
       </c>
       <c r="O135" t="inlineStr">
         <is>
@@ -12848,15 +12848,15 @@
         </is>
       </c>
       <c r="P135" t="n">
-        <v>3.52</v>
+        <v>3.22</v>
       </c>
       <c r="Q135" t="inlineStr">
         <is>
-          <t>08/10/2023 12:26</t>
+          <t>08/10/2023 13:53</t>
         </is>
       </c>
       <c r="R135" t="n">
-        <v>2.31</v>
+        <v>3.02</v>
       </c>
       <c r="S135" t="inlineStr">
         <is>
@@ -12864,16 +12864,16 @@
         </is>
       </c>
       <c r="T135" t="n">
-        <v>2.27</v>
+        <v>3.8</v>
       </c>
       <c r="U135" t="inlineStr">
         <is>
-          <t>08/10/2023 13:51</t>
+          <t>08/10/2023 13:53</t>
         </is>
       </c>
       <c r="V135" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/fc-bhayangkara-bali-united/neDqACL1/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-persik-kediri/QuPzCYjk/</t>
         </is>
       </c>
     </row>
@@ -14005,22 +14005,22 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>Persib Bandung</t>
+          <t>Borneo</t>
         </is>
       </c>
       <c r="G148" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>PSS Sleman</t>
+          <t>Dewa United</t>
         </is>
       </c>
       <c r="I148" t="n">
         <v>1</v>
       </c>
       <c r="J148" t="n">
-        <v>1.35</v>
+        <v>1.74</v>
       </c>
       <c r="K148" t="inlineStr">
         <is>
@@ -14028,15 +14028,15 @@
         </is>
       </c>
       <c r="L148" t="n">
-        <v>1.38</v>
+        <v>1.59</v>
       </c>
       <c r="M148" t="inlineStr">
         <is>
-          <t>28/10/2023 13:58</t>
+          <t>28/10/2023 13:21</t>
         </is>
       </c>
       <c r="N148" t="n">
-        <v>4.75</v>
+        <v>3.61</v>
       </c>
       <c r="O148" t="inlineStr">
         <is>
@@ -14044,15 +14044,15 @@
         </is>
       </c>
       <c r="P148" t="n">
-        <v>4.66</v>
+        <v>3.99</v>
       </c>
       <c r="Q148" t="inlineStr">
         <is>
-          <t>28/10/2023 13:58</t>
+          <t>28/10/2023 13:21</t>
         </is>
       </c>
       <c r="R148" t="n">
-        <v>6.7</v>
+        <v>4.2</v>
       </c>
       <c r="S148" t="inlineStr">
         <is>
@@ -14060,16 +14060,16 @@
         </is>
       </c>
       <c r="T148" t="n">
-        <v>8.380000000000001</v>
+        <v>5.64</v>
       </c>
       <c r="U148" t="inlineStr">
         <is>
-          <t>28/10/2023 13:58</t>
+          <t>28/10/2023 13:21</t>
         </is>
       </c>
       <c r="V148" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persib-bandung-pss-sleman/OfVQLizK/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-dewa-united/KQGdGVcs/</t>
         </is>
       </c>
     </row>
@@ -14097,22 +14097,22 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>Borneo</t>
+          <t>Persib Bandung</t>
         </is>
       </c>
       <c r="G149" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>Dewa United</t>
+          <t>PSS Sleman</t>
         </is>
       </c>
       <c r="I149" t="n">
         <v>1</v>
       </c>
       <c r="J149" t="n">
-        <v>1.74</v>
+        <v>1.35</v>
       </c>
       <c r="K149" t="inlineStr">
         <is>
@@ -14120,15 +14120,15 @@
         </is>
       </c>
       <c r="L149" t="n">
-        <v>1.59</v>
+        <v>1.38</v>
       </c>
       <c r="M149" t="inlineStr">
         <is>
-          <t>28/10/2023 13:21</t>
+          <t>28/10/2023 13:58</t>
         </is>
       </c>
       <c r="N149" t="n">
-        <v>3.61</v>
+        <v>4.75</v>
       </c>
       <c r="O149" t="inlineStr">
         <is>
@@ -14136,15 +14136,15 @@
         </is>
       </c>
       <c r="P149" t="n">
-        <v>3.99</v>
+        <v>4.66</v>
       </c>
       <c r="Q149" t="inlineStr">
         <is>
-          <t>28/10/2023 13:21</t>
+          <t>28/10/2023 13:58</t>
         </is>
       </c>
       <c r="R149" t="n">
-        <v>4.2</v>
+        <v>6.7</v>
       </c>
       <c r="S149" t="inlineStr">
         <is>
@@ -14152,16 +14152,16 @@
         </is>
       </c>
       <c r="T149" t="n">
-        <v>5.64</v>
+        <v>8.380000000000001</v>
       </c>
       <c r="U149" t="inlineStr">
         <is>
-          <t>28/10/2023 13:21</t>
+          <t>28/10/2023 13:58</t>
         </is>
       </c>
       <c r="V149" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/borneo-dewa-united/KQGdGVcs/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persib-bandung-pss-sleman/OfVQLizK/</t>
         </is>
       </c>
     </row>
@@ -15569,22 +15569,22 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>PSIS Semarang</t>
+          <t>Barito Putera</t>
         </is>
       </c>
       <c r="G165" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H165" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>Persebaya</t>
         </is>
       </c>
       <c r="I165" t="n">
         <v>0</v>
       </c>
       <c r="J165" t="n">
-        <v>1.66</v>
+        <v>1.93</v>
       </c>
       <c r="K165" t="inlineStr">
         <is>
@@ -15592,15 +15592,15 @@
         </is>
       </c>
       <c r="L165" t="n">
-        <v>1.52</v>
+        <v>1.85</v>
       </c>
       <c r="M165" t="inlineStr">
         <is>
-          <t>09/11/2023 08:57</t>
+          <t>09/11/2023 08:50</t>
         </is>
       </c>
       <c r="N165" t="n">
-        <v>3.56</v>
+        <v>3.49</v>
       </c>
       <c r="O165" t="inlineStr">
         <is>
@@ -15608,15 +15608,15 @@
         </is>
       </c>
       <c r="P165" t="n">
-        <v>4.06</v>
+        <v>3.42</v>
       </c>
       <c r="Q165" t="inlineStr">
         <is>
-          <t>09/11/2023 08:58</t>
+          <t>09/11/2023 08:59</t>
         </is>
       </c>
       <c r="R165" t="n">
-        <v>4.77</v>
+        <v>3.47</v>
       </c>
       <c r="S165" t="inlineStr">
         <is>
@@ -15624,16 +15624,16 @@
         </is>
       </c>
       <c r="T165" t="n">
-        <v>6.53</v>
+        <v>4.56</v>
       </c>
       <c r="U165" t="inlineStr">
         <is>
-          <t>09/11/2023 08:57</t>
+          <t>09/11/2023 08:59</t>
         </is>
       </c>
       <c r="V165" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/psis-semarang-persita/WtWvnllP/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-persebaya/UyhdN4BO/</t>
         </is>
       </c>
     </row>
@@ -15661,22 +15661,22 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Barito Putera</t>
+          <t>PSIS Semarang</t>
         </is>
       </c>
       <c r="G166" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H166" t="inlineStr">
         <is>
-          <t>Persebaya</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="I166" t="n">
         <v>0</v>
       </c>
       <c r="J166" t="n">
-        <v>1.93</v>
+        <v>1.66</v>
       </c>
       <c r="K166" t="inlineStr">
         <is>
@@ -15684,15 +15684,15 @@
         </is>
       </c>
       <c r="L166" t="n">
-        <v>1.85</v>
+        <v>1.52</v>
       </c>
       <c r="M166" t="inlineStr">
         <is>
-          <t>09/11/2023 08:50</t>
+          <t>09/11/2023 08:57</t>
         </is>
       </c>
       <c r="N166" t="n">
-        <v>3.49</v>
+        <v>3.56</v>
       </c>
       <c r="O166" t="inlineStr">
         <is>
@@ -15700,15 +15700,15 @@
         </is>
       </c>
       <c r="P166" t="n">
-        <v>3.42</v>
+        <v>4.06</v>
       </c>
       <c r="Q166" t="inlineStr">
         <is>
-          <t>09/11/2023 08:59</t>
+          <t>09/11/2023 08:58</t>
         </is>
       </c>
       <c r="R166" t="n">
-        <v>3.47</v>
+        <v>4.77</v>
       </c>
       <c r="S166" t="inlineStr">
         <is>
@@ -15716,16 +15716,16 @@
         </is>
       </c>
       <c r="T166" t="n">
-        <v>4.56</v>
+        <v>6.53</v>
       </c>
       <c r="U166" t="inlineStr">
         <is>
-          <t>09/11/2023 08:59</t>
+          <t>09/11/2023 08:57</t>
         </is>
       </c>
       <c r="V166" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-persebaya/UyhdN4BO/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/psis-semarang-persita/WtWvnllP/</t>
         </is>
       </c>
     </row>
@@ -16213,7 +16213,7 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>Persita</t>
+          <t>PSM Makassar</t>
         </is>
       </c>
       <c r="G172" t="n">
@@ -16221,14 +16221,14 @@
       </c>
       <c r="H172" t="inlineStr">
         <is>
-          <t>RANS Nusantara</t>
+          <t>Persikabo 1973</t>
         </is>
       </c>
       <c r="I172" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J172" t="n">
-        <v>2.09</v>
+        <v>1.44</v>
       </c>
       <c r="K172" t="inlineStr">
         <is>
@@ -16236,15 +16236,15 @@
         </is>
       </c>
       <c r="L172" t="n">
-        <v>2.59</v>
+        <v>1.38</v>
       </c>
       <c r="M172" t="inlineStr">
         <is>
-          <t>23/11/2023 12:59</t>
+          <t>23/11/2023 12:55</t>
         </is>
       </c>
       <c r="N172" t="n">
-        <v>3.31</v>
+        <v>4.32</v>
       </c>
       <c r="O172" t="inlineStr">
         <is>
@@ -16252,15 +16252,15 @@
         </is>
       </c>
       <c r="P172" t="n">
-        <v>3.59</v>
+        <v>4.97</v>
       </c>
       <c r="Q172" t="inlineStr">
         <is>
-          <t>23/11/2023 12:59</t>
+          <t>23/11/2023 12:55</t>
         </is>
       </c>
       <c r="R172" t="n">
-        <v>3.11</v>
+        <v>5.72</v>
       </c>
       <c r="S172" t="inlineStr">
         <is>
@@ -16268,16 +16268,16 @@
         </is>
       </c>
       <c r="T172" t="n">
-        <v>2.54</v>
+        <v>7.53</v>
       </c>
       <c r="U172" t="inlineStr">
         <is>
-          <t>23/11/2023 12:59</t>
+          <t>23/11/2023 12:55</t>
         </is>
       </c>
       <c r="V172" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-rans-nusantara/GnTQxpBB/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/psm-makassar-persikabo-1973/MPTMwQe5/</t>
         </is>
       </c>
     </row>
@@ -16305,7 +16305,7 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>PSM Makassar</t>
+          <t>Persita</t>
         </is>
       </c>
       <c r="G173" t="n">
@@ -16313,14 +16313,14 @@
       </c>
       <c r="H173" t="inlineStr">
         <is>
-          <t>Persikabo 1973</t>
+          <t>RANS Nusantara</t>
         </is>
       </c>
       <c r="I173" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J173" t="n">
-        <v>1.44</v>
+        <v>2.09</v>
       </c>
       <c r="K173" t="inlineStr">
         <is>
@@ -16328,15 +16328,15 @@
         </is>
       </c>
       <c r="L173" t="n">
-        <v>1.38</v>
+        <v>2.59</v>
       </c>
       <c r="M173" t="inlineStr">
         <is>
-          <t>23/11/2023 12:55</t>
+          <t>23/11/2023 12:59</t>
         </is>
       </c>
       <c r="N173" t="n">
-        <v>4.32</v>
+        <v>3.31</v>
       </c>
       <c r="O173" t="inlineStr">
         <is>
@@ -16344,15 +16344,15 @@
         </is>
       </c>
       <c r="P173" t="n">
-        <v>4.97</v>
+        <v>3.59</v>
       </c>
       <c r="Q173" t="inlineStr">
         <is>
-          <t>23/11/2023 12:55</t>
+          <t>23/11/2023 12:59</t>
         </is>
       </c>
       <c r="R173" t="n">
-        <v>5.72</v>
+        <v>3.11</v>
       </c>
       <c r="S173" t="inlineStr">
         <is>
@@ -16360,16 +16360,16 @@
         </is>
       </c>
       <c r="T173" t="n">
-        <v>7.53</v>
+        <v>2.54</v>
       </c>
       <c r="U173" t="inlineStr">
         <is>
-          <t>23/11/2023 12:55</t>
+          <t>23/11/2023 12:59</t>
         </is>
       </c>
       <c r="V173" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/indonesia/liga-1/psm-makassar-persikabo-1973/MPTMwQe5/</t>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persita-rans-nusantara/GnTQxpBB/</t>
         </is>
       </c>
     </row>
@@ -16922,6 +16922,190 @@
       <c r="V179" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/indonesia/liga-1/rans-nusantara-persebaya/6uEAxyHS/</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>indonesia</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>liga-1</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E180" s="2" t="n">
+        <v>45262.375</v>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>Persik Kediri</t>
+        </is>
+      </c>
+      <c r="G180" t="n">
+        <v>0</v>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>Dewa United</t>
+        </is>
+      </c>
+      <c r="I180" t="n">
+        <v>0</v>
+      </c>
+      <c r="J180" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>30/11/2023 21:13</t>
+        </is>
+      </c>
+      <c r="L180" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="M180" t="inlineStr">
+        <is>
+          <t>02/12/2023 08:57</t>
+        </is>
+      </c>
+      <c r="N180" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="O180" t="inlineStr">
+        <is>
+          <t>30/11/2023 21:13</t>
+        </is>
+      </c>
+      <c r="P180" t="n">
+        <v>3.86</v>
+      </c>
+      <c r="Q180" t="inlineStr">
+        <is>
+          <t>02/12/2023 08:57</t>
+        </is>
+      </c>
+      <c r="R180" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="S180" t="inlineStr">
+        <is>
+          <t>30/11/2023 21:13</t>
+        </is>
+      </c>
+      <c r="T180" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="U180" t="inlineStr">
+        <is>
+          <t>02/12/2023 08:57</t>
+        </is>
+      </c>
+      <c r="V180" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/persik-kediri-dewa-united/OGO5wH1M/</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>indonesia</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>liga-1</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E181" s="2" t="n">
+        <v>45262.375</v>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>Barito Putera</t>
+        </is>
+      </c>
+      <c r="G181" t="n">
+        <v>0</v>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>Borneo</t>
+        </is>
+      </c>
+      <c r="I181" t="n">
+        <v>0</v>
+      </c>
+      <c r="J181" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>30/11/2023 21:13</t>
+        </is>
+      </c>
+      <c r="L181" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="M181" t="inlineStr">
+        <is>
+          <t>02/12/2023 08:57</t>
+        </is>
+      </c>
+      <c r="N181" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="O181" t="inlineStr">
+        <is>
+          <t>30/11/2023 21:13</t>
+        </is>
+      </c>
+      <c r="P181" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="Q181" t="inlineStr">
+        <is>
+          <t>02/12/2023 08:58</t>
+        </is>
+      </c>
+      <c r="R181" t="n">
+        <v>2.37</v>
+      </c>
+      <c r="S181" t="inlineStr">
+        <is>
+          <t>30/11/2023 21:13</t>
+        </is>
+      </c>
+      <c r="T181" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="U181" t="inlineStr">
+        <is>
+          <t>02/12/2023 08:58</t>
+        </is>
+      </c>
+      <c r="V181" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/indonesia/liga-1/ps-barito-putera-borneo/r15xYfPq/</t>
         </is>
       </c>
     </row>

</xml_diff>